<commit_message>
Update README, map spreadsheet, & some minor edits to kastle_wood_device script
</commit_message>
<xml_diff>
--- a/Krieger Kastle.xlsx
+++ b/Krieger Kastle.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
   <si>
     <t>
 </t>
@@ -71,6 +71,9 @@
     <t>Weekly Spyglass</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>fish, water in pond</t>
   </si>
   <si>
@@ -104,9 +107,6 @@
     <t>Chuck (human)</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>ignition, steering wheel, cassette deck</t>
   </si>
   <si>
@@ -128,7 +128,7 @@
     <t>Krieger (human)</t>
   </si>
   <si>
-    <t>Near 43 may explode, move quickly</t>
+    <t>43 Requires Bomb to go south</t>
   </si>
   <si>
     <t>wooden device with wheel</t>
@@ -188,7 +188,7 @@
     <t>Death if you walk here</t>
   </si>
   <si>
-    <t>robot leg</t>
+    <t>used to be where 'A' is, but that is just an airlock ...</t>
   </si>
   <si>
     <t>Big Robot</t>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>the lab door on the west wall of 12 requires keycard from 43 to open</t>
+  </si>
+  <si>
+    <t>robot leg</t>
   </si>
   <si>
     <t>use the hand truck from 42 to haul the computer from 21 to 42 and use the data tape</t>
@@ -313,7 +316,7 @@
     </font>
     <font/>
     <font>
-      <sz val="15.0"/>
+      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -536,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="113">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -658,6 +661,9 @@
       <alignment/>
     </xf>
     <xf borderId="7" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="3" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
@@ -730,13 +736,7 @@
       <alignment/>
     </xf>
     <xf borderId="1" fillId="11" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="7" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -745,7 +745,7 @@
     <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="7" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -787,7 +787,7 @@
     <xf borderId="5" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="12" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -812,9 +812,6 @@
       <alignment/>
     </xf>
     <xf borderId="13" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="7" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -872,7 +869,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="35" width="3.29"/>
-    <col customWidth="1" min="36" max="36" width="41.29"/>
+    <col customWidth="1" min="36" max="36" width="43.43"/>
     <col customWidth="1" min="37" max="46" width="3.29"/>
   </cols>
   <sheetData>
@@ -1809,15 +1806,15 @@
       <c r="J18" s="32">
         <v>39.0</v>
       </c>
-      <c r="K18" s="38">
-        <v>35.0</v>
+      <c r="K18" s="41" t="s">
+        <v>19</v>
       </c>
       <c r="L18" s="16"/>
-      <c r="M18" s="41">
+      <c r="M18" s="42">
         <v>38.0</v>
       </c>
-      <c r="N18" s="42"/>
-      <c r="O18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="44"/>
       <c r="P18" s="16"/>
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
@@ -1841,7 +1838,7 @@
         <v>16.0</v>
       </c>
       <c r="AJ18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
@@ -1863,27 +1860,27 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="44"/>
+      <c r="I19" s="45"/>
       <c r="J19" s="16"/>
       <c r="K19" s="39" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="44"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="26"/>
       <c r="R19" s="13"/>
-      <c r="S19" s="45">
+      <c r="S19" s="46">
         <v>18.0</v>
       </c>
       <c r="T19" s="16"/>
-      <c r="U19" s="45">
+      <c r="U19" s="46">
         <v>18.0</v>
       </c>
       <c r="V19" s="13"/>
-      <c r="W19" s="45">
+      <c r="W19" s="46">
         <v>22.0</v>
       </c>
       <c r="X19" s="26"/>
@@ -1901,7 +1898,7 @@
         <v>17.0</v>
       </c>
       <c r="AJ19" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AK19" s="2"/>
       <c r="AL19" s="2"/>
@@ -1923,31 +1920,31 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="46">
+      <c r="I20" s="47">
         <v>40.0</v>
       </c>
       <c r="J20" s="16"/>
-      <c r="K20" s="47"/>
+      <c r="K20" s="48"/>
       <c r="L20" s="40"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="50"/>
       <c r="O20" s="37"/>
       <c r="P20" s="16"/>
-      <c r="Q20" s="50">
+      <c r="Q20" s="51">
         <v>11.0</v>
       </c>
-      <c r="R20" s="51"/>
-      <c r="S20" s="52">
+      <c r="R20" s="52"/>
+      <c r="S20" s="53">
         <v>13.0</v>
       </c>
       <c r="T20" s="16"/>
-      <c r="U20" s="53">
+      <c r="U20" s="54">
         <v>18.0</v>
       </c>
-      <c r="V20" s="53">
+      <c r="V20" s="54">
         <v>19.0</v>
       </c>
-      <c r="W20" s="53">
+      <c r="W20" s="54">
         <v>20.0</v>
       </c>
       <c r="X20" s="22"/>
@@ -1965,7 +1962,7 @@
         <v>18.0</v>
       </c>
       <c r="AJ20" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AK20" s="2"/>
       <c r="AL20" s="2"/>
@@ -1980,8 +1977,8 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="B21" s="54" t="s">
-        <v>23</v>
+      <c r="B21" s="55" t="s">
+        <v>24</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1989,11 +1986,11 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="44"/>
       <c r="N21" s="26"/>
       <c r="O21" s="26"/>
       <c r="P21" s="16"/>
@@ -2019,7 +2016,7 @@
         <v>19.0</v>
       </c>
       <c r="AJ21" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AK21" s="2"/>
       <c r="AL21" s="2"/>
@@ -2035,7 +2032,7 @@
     <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2046,8 +2043,8 @@
       <c r="I22" s="9"/>
       <c r="J22" s="16"/>
       <c r="K22" s="39"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="55">
+      <c r="L22" s="43"/>
+      <c r="M22" s="56">
         <v>8.0</v>
       </c>
       <c r="N22" s="19"/>
@@ -2058,16 +2055,16 @@
       <c r="Q22" s="14"/>
       <c r="R22" s="16"/>
       <c r="S22" s="24"/>
-      <c r="T22" s="56">
+      <c r="T22" s="57">
         <v>15.0</v>
       </c>
       <c r="U22" s="36">
         <v>16.0</v>
       </c>
       <c r="V22" s="16"/>
-      <c r="W22" s="57"/>
-      <c r="X22" s="58"/>
-      <c r="Y22" s="59"/>
+      <c r="W22" s="58"/>
+      <c r="X22" s="59"/>
+      <c r="Y22" s="60"/>
       <c r="Z22" s="16"/>
       <c r="AA22" s="36">
         <v>21.0</v>
@@ -2085,7 +2082,7 @@
         <v>20.0</v>
       </c>
       <c r="AJ22" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
@@ -2101,7 +2098,7 @@
     <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2112,7 +2109,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="16"/>
       <c r="K23" s="39"/>
-      <c r="L23" s="42"/>
+      <c r="L23" s="43"/>
       <c r="M23" s="26"/>
       <c r="N23" s="16"/>
       <c r="O23" s="15">
@@ -2125,9 +2122,9 @@
       <c r="T23" s="9"/>
       <c r="U23" s="26"/>
       <c r="V23" s="13"/>
-      <c r="W23" s="59"/>
+      <c r="W23" s="60"/>
       <c r="X23" s="16"/>
-      <c r="Y23" s="59"/>
+      <c r="Y23" s="60"/>
       <c r="Z23" s="26"/>
       <c r="AA23" s="26"/>
       <c r="AB23" s="16"/>
@@ -2141,7 +2138,7 @@
         <v>21.0</v>
       </c>
       <c r="AJ23" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
@@ -2157,7 +2154,7 @@
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2167,11 +2164,11 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="16"/>
-      <c r="K24" s="60" t="s">
-        <v>30</v>
+      <c r="K24" s="61" t="s">
+        <v>19</v>
       </c>
-      <c r="L24" s="61"/>
-      <c r="M24" s="62"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="63"/>
       <c r="N24" s="40"/>
       <c r="O24" s="19"/>
       <c r="P24" s="19"/>
@@ -2179,13 +2176,13 @@
       <c r="R24" s="19"/>
       <c r="S24" s="37"/>
       <c r="T24" s="16"/>
-      <c r="U24" s="57"/>
-      <c r="V24" s="58"/>
-      <c r="W24" s="63"/>
+      <c r="U24" s="58"/>
+      <c r="V24" s="59"/>
+      <c r="W24" s="64"/>
       <c r="X24" s="16"/>
-      <c r="Y24" s="58"/>
-      <c r="Z24" s="58"/>
-      <c r="AA24" s="59"/>
+      <c r="Y24" s="59"/>
+      <c r="Z24" s="59"/>
+      <c r="AA24" s="60"/>
       <c r="AB24" s="16"/>
       <c r="AC24" s="15">
         <v>25.0</v>
@@ -2228,7 +2225,7 @@
       <c r="K25" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="42"/>
+      <c r="L25" s="43"/>
       <c r="M25" s="26"/>
       <c r="N25" s="26"/>
       <c r="O25" s="26"/>
@@ -2237,13 +2234,13 @@
       <c r="R25" s="9"/>
       <c r="S25" s="26"/>
       <c r="T25" s="13"/>
-      <c r="U25" s="59"/>
+      <c r="U25" s="60"/>
       <c r="V25" s="9"/>
       <c r="W25" s="26"/>
       <c r="X25" s="26"/>
       <c r="Y25" s="26"/>
       <c r="Z25" s="13"/>
-      <c r="AA25" s="64">
+      <c r="AA25" s="65">
         <v>27.0</v>
       </c>
       <c r="AB25" s="13"/>
@@ -2285,29 +2282,29 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="16"/>
-      <c r="K26" s="65" t="s">
-        <v>30</v>
+      <c r="K26" s="66" t="s">
+        <v>19</v>
       </c>
-      <c r="L26" s="61"/>
-      <c r="M26" s="62"/>
-      <c r="N26" s="62"/>
-      <c r="O26" s="62"/>
-      <c r="P26" s="66"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
+      <c r="P26" s="67"/>
       <c r="Q26" s="15">
         <v>12.0</v>
       </c>
       <c r="R26" s="16"/>
-      <c r="S26" s="67"/>
-      <c r="T26" s="68"/>
-      <c r="U26" s="63"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="64"/>
       <c r="V26" s="16"/>
-      <c r="W26" s="58"/>
-      <c r="X26" s="58"/>
-      <c r="Y26" s="58"/>
-      <c r="Z26" s="58"/>
-      <c r="AA26" s="58"/>
-      <c r="AB26" s="58"/>
-      <c r="AC26" s="63"/>
+      <c r="W26" s="59"/>
+      <c r="X26" s="59"/>
+      <c r="Y26" s="59"/>
+      <c r="Z26" s="59"/>
+      <c r="AA26" s="59"/>
+      <c r="AB26" s="59"/>
+      <c r="AC26" s="64"/>
       <c r="AD26" s="17"/>
       <c r="AE26" s="9"/>
       <c r="AF26" s="2"/>
@@ -2344,24 +2341,24 @@
       <c r="I27" s="2"/>
       <c r="J27" s="16"/>
       <c r="K27" s="39"/>
-      <c r="L27" s="42"/>
+      <c r="L27" s="43"/>
       <c r="M27" s="26"/>
       <c r="N27" s="9"/>
       <c r="O27" s="26"/>
       <c r="P27" s="13"/>
       <c r="Q27" s="14"/>
       <c r="R27" s="9"/>
-      <c r="S27" s="69">
+      <c r="S27" s="68">
         <v>43.0</v>
       </c>
       <c r="T27" s="9"/>
-      <c r="U27" s="70" t="s">
+      <c r="U27" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="V27" s="42"/>
-      <c r="W27" s="42"/>
-      <c r="X27" s="42"/>
-      <c r="Y27" s="42"/>
+      <c r="V27" s="43"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="43"/>
+      <c r="Y27" s="43"/>
       <c r="Z27" s="9"/>
       <c r="AA27" s="9"/>
       <c r="AB27" s="9"/>
@@ -2401,9 +2398,11 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="16"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="71">
+      <c r="K28" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28" s="62"/>
+      <c r="M28" s="70">
         <v>42.0</v>
       </c>
       <c r="N28" s="40"/>
@@ -2413,19 +2412,19 @@
       <c r="P28" s="19"/>
       <c r="Q28" s="37"/>
       <c r="R28" s="9"/>
-      <c r="S28" s="72"/>
+      <c r="S28" s="71"/>
       <c r="T28" s="9"/>
-      <c r="U28" s="73"/>
-      <c r="V28" s="74"/>
-      <c r="W28" s="74"/>
-      <c r="X28" s="75">
+      <c r="U28" s="72"/>
+      <c r="V28" s="73"/>
+      <c r="W28" s="73"/>
+      <c r="X28" s="74">
         <v>51.0</v>
       </c>
-      <c r="Y28" s="76"/>
-      <c r="Z28" s="77"/>
-      <c r="AA28" s="78"/>
-      <c r="AB28" s="77"/>
-      <c r="AC28" s="79"/>
+      <c r="Y28" s="75"/>
+      <c r="Z28" s="76"/>
+      <c r="AA28" s="77"/>
+      <c r="AB28" s="76"/>
+      <c r="AC28" s="78"/>
       <c r="AD28" s="17"/>
       <c r="AE28" s="9"/>
       <c r="AF28" s="2"/>
@@ -2434,7 +2433,7 @@
       <c r="AI28" s="5">
         <v>26.0</v>
       </c>
-      <c r="AJ28" s="80" t="s">
+      <c r="AJ28" s="79" t="s">
         <v>41</v>
       </c>
       <c r="AK28" s="2"/>
@@ -2464,24 +2463,24 @@
       <c r="K29" s="38">
         <v>41.0</v>
       </c>
-      <c r="L29" s="42"/>
+      <c r="L29" s="43"/>
       <c r="M29" s="26"/>
       <c r="N29" s="13"/>
       <c r="O29" s="14"/>
       <c r="P29" s="9"/>
       <c r="Q29" s="9"/>
       <c r="R29" s="9"/>
-      <c r="S29" s="72"/>
+      <c r="S29" s="71"/>
       <c r="T29" s="9"/>
-      <c r="U29" s="81"/>
+      <c r="U29" s="80"/>
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
-      <c r="X29" s="42"/>
-      <c r="Y29" s="82"/>
+      <c r="X29" s="43"/>
+      <c r="Y29" s="81"/>
       <c r="Z29" s="9"/>
-      <c r="AA29" s="81"/>
+      <c r="AA29" s="80"/>
       <c r="AB29" s="9"/>
-      <c r="AC29" s="83">
+      <c r="AC29" s="82">
         <v>52.0</v>
       </c>
       <c r="AD29" s="17"/>
@@ -2517,33 +2516,33 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="16"/>
-      <c r="K30" s="84"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="85"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="84"/>
       <c r="N30" s="19"/>
       <c r="O30" s="37"/>
       <c r="P30" s="9"/>
-      <c r="Q30" s="86"/>
-      <c r="R30" s="87"/>
-      <c r="S30" s="88">
+      <c r="Q30" s="85"/>
+      <c r="R30" s="86"/>
+      <c r="S30" s="87">
         <v>46.0</v>
       </c>
       <c r="T30" s="9"/>
-      <c r="U30" s="83">
+      <c r="U30" s="82">
         <v>48.0</v>
       </c>
       <c r="V30" s="9"/>
-      <c r="W30" s="89">
+      <c r="W30" s="88">
         <v>50.0</v>
       </c>
-      <c r="X30" s="42"/>
-      <c r="Y30" s="90">
+      <c r="X30" s="43"/>
+      <c r="Y30" s="89">
         <v>53.0</v>
       </c>
-      <c r="Z30" s="42"/>
-      <c r="AA30" s="82"/>
+      <c r="Z30" s="43"/>
+      <c r="AA30" s="81"/>
       <c r="AB30" s="9"/>
-      <c r="AC30" s="91">
+      <c r="AC30" s="90">
         <v>54.0</v>
       </c>
       <c r="AD30" s="17"/>
@@ -2587,21 +2586,21 @@
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
-      <c r="Q31" s="92"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="42"/>
-      <c r="T31" s="42"/>
-      <c r="U31" s="83"/>
+      <c r="Q31" s="91"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
+      <c r="T31" s="43"/>
+      <c r="U31" s="82"/>
       <c r="V31" s="9"/>
-      <c r="W31" s="83">
+      <c r="W31" s="82">
         <v>49.0</v>
       </c>
-      <c r="X31" s="42"/>
-      <c r="Y31" s="93" t="s">
+      <c r="X31" s="43"/>
+      <c r="Y31" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="Z31" s="42"/>
-      <c r="AA31" s="82"/>
+      <c r="Z31" s="43"/>
+      <c r="AA31" s="81"/>
       <c r="AB31" s="9"/>
       <c r="AC31" s="9"/>
       <c r="AD31" s="9"/>
@@ -2640,25 +2639,25 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
-      <c r="O32" s="86">
+      <c r="O32" s="85">
         <v>47.0</v>
       </c>
-      <c r="P32" s="87"/>
-      <c r="Q32" s="94"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="95"/>
-      <c r="T32" s="74"/>
-      <c r="U32" s="96"/>
-      <c r="V32" s="74"/>
-      <c r="W32" s="97"/>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="42"/>
-      <c r="Z32" s="42"/>
-      <c r="AA32" s="98"/>
-      <c r="AB32" s="99">
+      <c r="P32" s="86"/>
+      <c r="Q32" s="93"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="94"/>
+      <c r="T32" s="73"/>
+      <c r="U32" s="95"/>
+      <c r="V32" s="73"/>
+      <c r="W32" s="96"/>
+      <c r="X32" s="43"/>
+      <c r="Y32" s="43"/>
+      <c r="Z32" s="43"/>
+      <c r="AA32" s="97"/>
+      <c r="AB32" s="98">
         <v>56.0</v>
       </c>
-      <c r="AC32" s="100"/>
+      <c r="AC32" s="99"/>
       <c r="AD32" s="17"/>
       <c r="AE32" s="9"/>
       <c r="AF32" s="2"/>
@@ -2696,18 +2695,18 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="9"/>
-      <c r="O33" s="101"/>
+      <c r="O33" s="71"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="9"/>
       <c r="R33" s="9"/>
-      <c r="S33" s="82"/>
-      <c r="T33" s="42"/>
-      <c r="U33" s="42"/>
-      <c r="V33" s="42"/>
-      <c r="W33" s="42"/>
-      <c r="X33" s="42"/>
-      <c r="Z33" s="42"/>
-      <c r="AA33" s="82"/>
+      <c r="S33" s="81"/>
+      <c r="T33" s="43"/>
+      <c r="U33" s="43"/>
+      <c r="V33" s="43"/>
+      <c r="W33" s="43"/>
+      <c r="X33" s="43"/>
+      <c r="Z33" s="43"/>
+      <c r="AA33" s="81"/>
       <c r="AB33" s="9"/>
       <c r="AC33" s="9"/>
       <c r="AD33" s="9"/>
@@ -2741,16 +2740,16 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="9"/>
-      <c r="O34" s="102"/>
-      <c r="P34" s="77"/>
-      <c r="Q34" s="77"/>
-      <c r="R34" s="77"/>
-      <c r="S34" s="97"/>
+      <c r="O34" s="100"/>
+      <c r="P34" s="76"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="76"/>
+      <c r="S34" s="96"/>
       <c r="T34" s="9"/>
-      <c r="Z34" s="42"/>
-      <c r="AA34" s="103"/>
-      <c r="AB34" s="77"/>
-      <c r="AC34" s="104">
+      <c r="Z34" s="43"/>
+      <c r="AA34" s="101"/>
+      <c r="AB34" s="76"/>
+      <c r="AC34" s="102">
         <v>55.0</v>
       </c>
       <c r="AD34" s="17"/>
@@ -2780,7 +2779,7 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>50</v>
@@ -2794,13 +2793,13 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="9"/>
-      <c r="O35" s="105" t="s">
+      <c r="O35" s="103" t="s">
         <v>51</v>
       </c>
       <c r="P35" s="17"/>
       <c r="Q35" s="17"/>
       <c r="R35" s="17"/>
-      <c r="S35" s="106"/>
+      <c r="S35" s="104"/>
       <c r="T35" s="9"/>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
@@ -2808,7 +2807,7 @@
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
       <c r="Z35" s="9"/>
-      <c r="AA35" s="105" t="s">
+      <c r="AA35" s="103" t="s">
         <v>52</v>
       </c>
       <c r="AB35" s="17"/>
@@ -2858,14 +2857,14 @@
       <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
       <c r="R36" s="9"/>
-      <c r="S36" s="42"/>
-      <c r="T36" s="42"/>
+      <c r="S36" s="43"/>
+      <c r="T36" s="43"/>
       <c r="V36" s="2"/>
       <c r="Y36" s="2"/>
       <c r="Z36" s="9"/>
       <c r="AA36" s="9"/>
       <c r="AB36" s="9"/>
-      <c r="AC36" s="42"/>
+      <c r="AC36" s="43"/>
       <c r="AD36" s="9"/>
       <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
@@ -2874,7 +2873,7 @@
       <c r="AI36" s="5">
         <v>34.0</v>
       </c>
-      <c r="AJ36" s="80" t="s">
+      <c r="AJ36" s="79" t="s">
         <v>55</v>
       </c>
       <c r="AK36" s="2"/>
@@ -2892,7 +2891,7 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>56</v>
@@ -2923,10 +2922,10 @@
       <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
-      <c r="AI37" s="107">
+      <c r="AI37" s="105">
         <v>35.0</v>
       </c>
-      <c r="AJ37" s="2" t="s">
+      <c r="AJ37" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK37" s="2"/>
@@ -2943,16 +2942,16 @@
     <row r="38" ht="13.5" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
-      <c r="D38" s="108" t="s">
+      <c r="D38" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="108" t="s">
+      <c r="E38" s="106" t="s">
         <v>59</v>
       </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
       <c r="V38" s="2"/>
-      <c r="W38" s="57"/>
+      <c r="W38" s="58"/>
       <c r="X38" s="4" t="s">
         <v>60</v>
       </c>
@@ -2966,7 +2965,7 @@
       <c r="AF38" s="2"/>
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
-      <c r="AI38" s="107">
+      <c r="AI38" s="105">
         <v>36.0</v>
       </c>
       <c r="AJ38" s="2" t="s">
@@ -2989,7 +2988,7 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
       <c r="V39" s="2"/>
-      <c r="W39" s="109"/>
+      <c r="W39" s="107"/>
       <c r="X39" s="4" t="s">
         <v>62</v>
       </c>
@@ -3002,7 +3001,7 @@
       <c r="AF39" s="2"/>
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
-      <c r="AI39" s="107">
+      <c r="AI39" s="105">
         <v>37.0</v>
       </c>
       <c r="AJ39" s="2" t="s">
@@ -3052,7 +3051,7 @@
       <c r="AF40" s="2"/>
       <c r="AG40" s="2"/>
       <c r="AH40" s="2"/>
-      <c r="AI40" s="107">
+      <c r="AI40" s="105">
         <v>38.0</v>
       </c>
       <c r="AJ40" s="2" t="s">
@@ -3091,7 +3090,7 @@
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
-      <c r="W41" s="110"/>
+      <c r="W41" s="108"/>
       <c r="X41" s="2" t="s">
         <v>66</v>
       </c>
@@ -3105,7 +3104,7 @@
       <c r="AF41" s="2"/>
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
-      <c r="AI41" s="107">
+      <c r="AI41" s="105">
         <v>39.0</v>
       </c>
       <c r="AJ41" s="2" t="s">
@@ -3144,7 +3143,7 @@
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
-      <c r="W42" s="111"/>
+      <c r="W42" s="109"/>
       <c r="X42" s="1" t="s">
         <v>68</v>
       </c>
@@ -3158,7 +3157,7 @@
       <c r="AF42" s="2"/>
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
-      <c r="AI42" s="107">
+      <c r="AI42" s="105">
         <v>40.0</v>
       </c>
       <c r="AJ42" s="2" t="s">
@@ -3193,7 +3192,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
-      <c r="S43" s="112" t="s">
+      <c r="S43" s="110" t="s">
         <v>70</v>
       </c>
       <c r="T43" s="2"/>
@@ -3211,7 +3210,7 @@
       <c r="AF43" s="2"/>
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
-      <c r="AI43" s="107">
+      <c r="AI43" s="105">
         <v>41.0</v>
       </c>
       <c r="AJ43" s="2" t="s">
@@ -3265,7 +3264,7 @@
       <c r="AF44" s="2"/>
       <c r="AG44" s="2"/>
       <c r="AH44" s="2"/>
-      <c r="AI44" s="107">
+      <c r="AI44" s="105">
         <v>42.0</v>
       </c>
       <c r="AJ44" s="1" t="s">
@@ -3319,7 +3318,7 @@
       <c r="AF45" s="2"/>
       <c r="AG45" s="2"/>
       <c r="AH45" s="2"/>
-      <c r="AI45" s="107">
+      <c r="AI45" s="105">
         <v>43.0</v>
       </c>
       <c r="AJ45" s="2" t="s">
@@ -3376,8 +3375,8 @@
       <c r="AI46" s="1">
         <v>44.0</v>
       </c>
-      <c r="AJ46" s="113" t="s">
-        <v>58</v>
+      <c r="AJ46" s="111" t="s">
+        <v>77</v>
       </c>
       <c r="AK46" s="2"/>
       <c r="AL46" s="2"/>
@@ -3392,7 +3391,7 @@
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3428,7 +3427,7 @@
       <c r="AG47" s="2"/>
       <c r="AH47" s="2"/>
       <c r="AI47" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
@@ -3444,7 +3443,7 @@
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3483,7 +3482,7 @@
         <v>46.0</v>
       </c>
       <c r="AJ48" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AK48" s="2"/>
       <c r="AL48" s="2"/>
@@ -3498,7 +3497,7 @@
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -3537,7 +3536,7 @@
         <v>47.0</v>
       </c>
       <c r="AJ49" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AK49" s="2"/>
       <c r="AL49" s="2"/>
@@ -3589,7 +3588,7 @@
         <v>48.0</v>
       </c>
       <c r="AJ50" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AK50" s="2"/>
       <c r="AL50" s="2"/>
@@ -3641,7 +3640,7 @@
         <v>49.0</v>
       </c>
       <c r="AJ51" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AK51" s="2"/>
       <c r="AL51" s="2"/>
@@ -3693,7 +3692,7 @@
         <v>50.0</v>
       </c>
       <c r="AJ52" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AK52" s="2"/>
       <c r="AL52" s="2"/>
@@ -3745,7 +3744,7 @@
         <v>51.0</v>
       </c>
       <c r="AJ53" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AR53" s="2"/>
       <c r="AS53" s="2"/>
@@ -3790,7 +3789,7 @@
         <v>52.0</v>
       </c>
       <c r="AJ54" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AR54" s="2"/>
       <c r="AS54" s="2"/>
@@ -3835,7 +3834,7 @@
         <v>53.0</v>
       </c>
       <c r="AJ55" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AK55" s="2"/>
       <c r="AL55" s="2"/>
@@ -3887,7 +3886,7 @@
         <v>54.0</v>
       </c>
       <c r="AJ56" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AR56" s="2"/>
       <c r="AS56" s="2"/>
@@ -3932,7 +3931,7 @@
         <v>55.0</v>
       </c>
       <c r="AJ57" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AO57" s="2"/>
       <c r="AP57" s="2"/>
@@ -3979,8 +3978,8 @@
       <c r="AI58" s="1">
         <v>56.0</v>
       </c>
-      <c r="AJ58" s="114" t="s">
-        <v>91</v>
+      <c r="AJ58" s="112" t="s">
+        <v>92</v>
       </c>
       <c r="AR58" s="2"/>
       <c r="AS58" s="2"/>

</xml_diff>

<commit_message>
Edit do function to take in disp_txt variable to control displaying output
</commit_message>
<xml_diff>
--- a/Krieger Kastle.xlsx
+++ b/Krieger Kastle.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>
 </t>
@@ -23,13 +23,13 @@
     <t>start, stick</t>
   </si>
   <si>
-    <t>META GAME</t>
+    <t>row of rocks arranged by size</t>
   </si>
   <si>
     <t>man eating plant, requires stick</t>
   </si>
   <si>
-    <t>Type 'quit'</t>
+    <t>little robot arm, Bucky</t>
   </si>
   <si>
     <t>diskette, chainsaw</t>
@@ -38,91 +38,94 @@
     <t>gas, key</t>
   </si>
   <si>
+    <t>pinata</t>
+  </si>
+  <si>
     <t>Door East, need key</t>
   </si>
   <si>
     <t>briefcase, muffin</t>
   </si>
   <si>
+    <t>beer bottle, console</t>
+  </si>
+  <si>
     <t>drum stick</t>
+  </si>
+  <si>
+    <t>slingshot</t>
   </si>
   <si>
     <t>torch</t>
   </si>
   <si>
+    <t>poster, crockpot, console</t>
+  </si>
+  <si>
     <t>glue bottle</t>
+  </si>
+  <si>
+    <t>stationary bike</t>
   </si>
   <si>
     <t>garrote</t>
   </si>
   <si>
+    <t>box, hand truck, console, data tape</t>
+  </si>
+  <si>
+    <t>characters:</t>
+  </si>
+  <si>
     <t>thermos</t>
+  </si>
+  <si>
+    <t>skeleton, rubble, keycard</t>
+  </si>
+  <si>
+    <t>Ed (human)</t>
   </si>
   <si>
     <t>staff room, dumpster, graffiti</t>
   </si>
   <si>
+    <t>robot leg</t>
+  </si>
+  <si>
+    <t>Bucky</t>
+  </si>
+  <si>
     <t>crumpled up paper</t>
+  </si>
+  <si>
+    <t>blood vials, punch card</t>
+  </si>
+  <si>
+    <t>Chuck (human)</t>
   </si>
   <si>
     <t>How To Archer Paperback</t>
   </si>
   <si>
+    <t>Poisocaine Pen</t>
+  </si>
+  <si>
+    <t>Rabbert</t>
+  </si>
+  <si>
     <t>Weekly Spyglass</t>
   </si>
   <si>
-    <t>A</t>
+    <t>Whiskey Stones</t>
+  </si>
+  <si>
+    <t>Milton</t>
   </si>
   <si>
     <t>fish, water in pond</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>Missing 2112 album</t>
-  </si>
-  <si>
-    <t>crumbs</t>
-  </si>
-  <si>
-    <t>characters:</t>
-  </si>
-  <si>
-    <t>hamburger</t>
-  </si>
-  <si>
-    <t>Ed (human)</t>
-  </si>
-  <si>
-    <t>glove compartment, manual, cassette, bottle cap</t>
-  </si>
-  <si>
-    <t>Bucky</t>
-  </si>
-  <si>
-    <t>computer, crevice</t>
-  </si>
-  <si>
-    <t>Chuck (human)</t>
-  </si>
-  <si>
-    <t>ignition, steering wheel, cassette deck</t>
-  </si>
-  <si>
-    <t>Rabbert</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>cesta</t>
-  </si>
-  <si>
-    <t>Milton</t>
-  </si>
-  <si>
-    <t>stack of flyers</t>
+    <t>Knife</t>
   </si>
   <si>
     <t>Krieger (human)</t>
@@ -131,40 +134,61 @@
     <t>43 Requires Bomb to go south</t>
   </si>
   <si>
-    <t>wooden device with wheel</t>
+    <t>Missing 2112 album</t>
+  </si>
+  <si>
+    <t>candy bar wrapper, modern art</t>
   </si>
   <si>
     <t>Bryan (human)</t>
   </si>
   <si>
-    <t>door, stick</t>
+    <t>crumbs</t>
+  </si>
+  <si>
+    <t>large foil swan</t>
   </si>
   <si>
     <t>Tim</t>
   </si>
   <si>
-    <t>Other Other Barry, need chainsaw or other</t>
+    <t>hamburger</t>
   </si>
   <si>
-    <t>gator tooth</t>
+    <t>Metal sculpture</t>
+  </si>
+  <si>
+    <t>glove box, manual, cassette, bottle cap</t>
+  </si>
+  <si>
+    <t>Compusave Multimedia Center</t>
   </si>
   <si>
     <t>R</t>
   </si>
   <si>
-    <t>bowling ball</t>
+    <t>computer, crevice</t>
   </si>
   <si>
-    <t>computer monitor in room, dim green</t>
+    <t>Knitting Needle</t>
   </si>
   <si>
-    <t>mare's leg, dry ice, cooler (can't pick up)</t>
+    <t>ignition, steering wheel, cassette deck</t>
   </si>
   <si>
-    <t>Deadly Velvet poster</t>
+    <t>Spatula, Little Hat</t>
   </si>
   <si>
-    <t>airlock</t>
+    <t>cesta</t>
+  </si>
+  <si>
+    <t>Bratwurst</t>
+  </si>
+  <si>
+    <t>stack of flyers</t>
+  </si>
+  <si>
+    <t>Laptop, Torn Paper (iyrwgknhuosgajpmjmaa)</t>
   </si>
   <si>
     <t>Can pickup "hole"</t>
@@ -173,13 +197,13 @@
     <t>window</t>
   </si>
   <si>
-    <t>row of rocks arranged by size</t>
+    <t>wooden device with wheel</t>
   </si>
   <si>
-    <t>tanning bed (using this will kill you)</t>
+    <t>tanning bed (using it kills you)</t>
   </si>
   <si>
-    <t>little robot arm, Bucky</t>
+    <t>door, stick</t>
   </si>
   <si>
     <t>game room (skeeball, token machine)</t>
@@ -188,7 +212,7 @@
     <t>Death if you walk here</t>
   </si>
   <si>
-    <t>used to be where 'A' is, but that is just an airlock ...</t>
+    <t>Other Other Barry, need chainsaw or other</t>
   </si>
   <si>
     <t>Big Robot</t>
@@ -197,107 +221,68 @@
     <t>Cave</t>
   </si>
   <si>
-    <t>pinata</t>
+    <t>gator tooth</t>
   </si>
   <si>
     <t>Van</t>
   </si>
   <si>
-    <t>punched card</t>
+    <t>bowling ball</t>
   </si>
   <si>
     <t>Jungle</t>
   </si>
   <si>
-    <t>beer bottle, console</t>
+    <t>computer monitor in room, dim green</t>
   </si>
   <si>
     <t>Lab</t>
   </si>
   <si>
-    <t>slingshot</t>
+    <t>mare's leg, dry ice, cooler (can't pick up)</t>
   </si>
   <si>
     <t>City</t>
   </si>
   <si>
-    <t>poster, crockpot, console</t>
+    <t>Deadly Velvet poster</t>
   </si>
   <si>
     <t>Everything else is mostly Krieger's Kastle or cliffs</t>
   </si>
   <si>
-    <t>stationary bike</t>
+    <t>you can construct a dry ice bomb with a bottle, water, dry ice, and bottlecap (fill bottle with water from pond at 16, 'use ice on beer', 'use cap on bomb', RUN)</t>
   </si>
   <si>
-    <t>you can construct a dry ice bomb with a bottle, water, dry ice, and bottlecap</t>
-  </si>
-  <si>
-    <t>box, hand truck, console, data tape</t>
-  </si>
-  <si>
-    <t>having three people hold down all three console buttons at 38/40/42 releases a murderous octopus from the cryo chamber</t>
-  </si>
-  <si>
-    <t>skeleton, rubble, keycard</t>
+    <t>having three people hold down all three console buttons at 38/40/42 releases a murderous octopus from the cryo chamber ('press button')</t>
   </si>
   <si>
     <t>the lab door on the west wall of 12 requires keycard from 43 to open</t>
   </si>
   <si>
-    <t>robot leg</t>
-  </si>
-  <si>
     <t>use the hand truck from 42 to haul the computer from 21 to 42 and use the data tape</t>
-  </si>
-  <si>
-    <t>45 blood vials, punch card</t>
   </si>
   <si>
     <t>Chuck and Bucky like to kill people.  Ed is friendly.</t>
   </si>
   <si>
-    <t>Poisocaine Pen</t>
+    <t>One person must hold the wheel at 25 for the door at 26 to be open, now automatically closes after about 5 seconds</t>
   </si>
   <si>
-    <t>one person must hold the wheel at 25 for the door at 26 to be open</t>
+    <t>43 requires dry ice bomb to get past, cave will cave in and kill you after a few seconds if you don't rush back by</t>
   </si>
   <si>
-    <t>Whiskey Stones</t>
+    <t>META GAME</t>
   </si>
   <si>
-    <t>Knife</t>
-  </si>
-  <si>
-    <t>candy bar wrapper, modern art</t>
-  </si>
-  <si>
-    <t>large foil swan</t>
-  </si>
-  <si>
-    <t>Metal sculpture</t>
-  </si>
-  <si>
-    <t>Compusave Multimedia Center</t>
-  </si>
-  <si>
-    <t>Knitting Needle</t>
-  </si>
-  <si>
-    <t>Spatula, Little Hat</t>
-  </si>
-  <si>
-    <t>Bratwurst</t>
-  </si>
-  <si>
-    <t>Laptop, Torn Paper (iyrwgknhuosgajpmjmaa)</t>
+    <t>Type 'quit'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -316,6 +301,10 @@
     </font>
     <font/>
     <font>
+      <color rgb="FF000000"/>
+      <name val="'Arial'"/>
+    </font>
+    <font>
       <sz val="10.0"/>
       <name val="Arial"/>
     </font>
@@ -329,18 +318,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
@@ -349,6 +326,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -397,6 +380,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB45F06"/>
         <bgColor rgb="FFB45F06"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -539,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -555,31 +544,25 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -588,13 +571,19 @@
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -603,28 +592,28 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -633,70 +622,73 @@
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="5" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="6" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="7" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="8" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -705,148 +697,151 @@
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="1" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="2" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="5" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="3" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="2" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="1" fillId="10" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="7" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="4" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="5" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="3" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="12" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="8" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="11" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="3" fillId="11" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="13" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="10" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="5" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="11" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="7" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="5" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="9" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="9" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="6" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="7" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="7" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="5" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="12" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="7" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="8" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="7" fillId="12" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="12" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="13" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="10" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -869,8 +864,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="35" width="3.29"/>
-    <col customWidth="1" min="36" max="36" width="43.43"/>
-    <col customWidth="1" min="37" max="46" width="3.29"/>
+    <col customWidth="1" min="36" max="36" width="35.86"/>
+    <col customWidth="1" min="37" max="37" width="3.0"/>
+    <col customWidth="1" min="38" max="38" width="43.43"/>
+    <col customWidth="1" min="39" max="46" width="3.29"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
@@ -981,152 +978,152 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
-      <c r="AI3" s="5">
+      <c r="AI3" s="6">
         <v>1.0</v>
       </c>
       <c r="AJ3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
+      <c r="AK3" s="6">
+        <v>33.0</v>
+      </c>
+      <c r="AL3" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="AT3" s="2"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
-      <c r="AI4" s="5">
+      <c r="AI4" s="6">
         <v>2.0</v>
       </c>
       <c r="AJ4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="2"/>
-      <c r="AM4" s="2"/>
-      <c r="AN4" s="2"/>
-      <c r="AO4" s="2"/>
-      <c r="AP4" s="2"/>
-      <c r="AQ4" s="2"/>
-      <c r="AR4" s="2"/>
-      <c r="AS4" s="2"/>
+      <c r="AK4" s="6">
+        <v>34.0</v>
+      </c>
+      <c r="AL4" s="8" t="s">
+        <v>5</v>
+      </c>
       <c r="AT4" s="2"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="2"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10">
+        <v>4.0</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="13">
+        <v>6.0</v>
+      </c>
+      <c r="N5" s="11"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="13">
+        <v>29.0</v>
+      </c>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="13">
+        <v>31.0</v>
+      </c>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="5"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
-      <c r="AI5" s="5">
+      <c r="AI5" s="6">
         <v>3.0</v>
       </c>
-      <c r="AJ5" s="8" t="s">
+      <c r="AJ5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="AK5" s="2"/>
-      <c r="AL5" s="2"/>
+      <c r="AK5" s="17">
+        <v>35.0</v>
+      </c>
+      <c r="AL5" s="1"/>
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
-      <c r="AO5" s="4"/>
+      <c r="AO5" s="2"/>
       <c r="AP5" s="2"/>
       <c r="AQ5" s="2"/>
       <c r="AR5" s="2"/>
@@ -1141,41 +1138,53 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21">
+        <v>5.0</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="23">
+        <v>34.0</v>
+      </c>
+      <c r="T6" s="14"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="13">
+        <v>32.0</v>
+      </c>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="5"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
-      <c r="AI6" s="5">
+      <c r="AI6" s="6">
         <v>4.0</v>
       </c>
       <c r="AJ6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AK6" s="2"/>
-      <c r="AL6" s="2"/>
+      <c r="AK6" s="17">
+        <v>36.0</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
       <c r="AO6" s="2"/>
@@ -1191,45 +1200,49 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="13">
+        <v>33.0</v>
+      </c>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="5"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
-      <c r="AI7" s="5">
+      <c r="AI7" s="6">
         <v>5.0</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
-      <c r="AK7" s="2"/>
+      <c r="AK7" s="17">
+        <v>37.0</v>
+      </c>
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
-      <c r="AN7" s="2"/>
+      <c r="AN7" s="1"/>
       <c r="AO7" s="2"/>
       <c r="AP7" s="2"/>
       <c r="AQ7" s="2"/>
@@ -1243,43 +1256,63 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="I8" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="32">
+        <v>36.0</v>
+      </c>
+      <c r="M8" s="33">
+        <v>45.0</v>
+      </c>
+      <c r="N8" s="14"/>
+      <c r="O8" s="13">
+        <v>7.0</v>
+      </c>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="34">
+        <v>28.0</v>
+      </c>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="36">
+        <v>30.0</v>
+      </c>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="34">
+        <v>23.0</v>
+      </c>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="27"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="37"/>
+      <c r="AD8" s="15"/>
+      <c r="AE8" s="5"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
-      <c r="AI8" s="5">
+      <c r="AI8" s="6">
         <v>6.0</v>
       </c>
       <c r="AJ8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
-      <c r="AK8" s="2"/>
-      <c r="AL8" s="2"/>
+      <c r="AK8" s="17">
+        <v>38.0</v>
+      </c>
+      <c r="AL8" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
@@ -1295,43 +1328,49 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="38">
+        <v>44.0</v>
+      </c>
+      <c r="L9" s="14"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
-      <c r="AI9" s="5">
+      <c r="AI9" s="6">
         <v>7.0</v>
       </c>
       <c r="AJ9" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
-      <c r="AK9" s="2"/>
-      <c r="AL9" s="2"/>
+      <c r="AK9" s="17">
+        <v>39.0</v>
+      </c>
+      <c r="AL9" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
       <c r="AO9" s="2"/>
@@ -1344,46 +1383,54 @@
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="32">
+        <v>39.0</v>
+      </c>
+      <c r="K10" s="41"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="42">
+        <v>38.0</v>
+      </c>
+      <c r="N10" s="43"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="35"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="5"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
-      <c r="AI10" s="5">
+      <c r="AI10" s="6">
         <v>8.0</v>
       </c>
       <c r="AJ10" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
-      <c r="AK10" s="2"/>
-      <c r="AL10" s="2"/>
+      <c r="AK10" s="17">
+        <v>40.0</v>
+      </c>
+      <c r="AL10" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
       <c r="AO10" s="2"/>
@@ -1396,46 +1443,58 @@
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="2"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="46">
+        <v>58.0</v>
+      </c>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="47">
+        <v>18.0</v>
+      </c>
+      <c r="T11" s="14"/>
+      <c r="U11" s="47">
+        <v>18.0</v>
+      </c>
+      <c r="V11" s="11"/>
+      <c r="W11" s="47">
+        <v>22.0</v>
+      </c>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="5"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
-      <c r="AI11" s="5">
+      <c r="AI11" s="6">
         <v>9.0</v>
       </c>
       <c r="AJ11" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
-      <c r="AK11" s="2"/>
-      <c r="AL11" s="2"/>
+      <c r="AK11" s="17">
+        <v>41.0</v>
+      </c>
+      <c r="AL11" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
       <c r="AO11" s="2"/>
@@ -1453,41 +1512,57 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="10"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="10"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="48">
+        <v>40.0</v>
+      </c>
+      <c r="J12" s="14"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="52">
+        <v>11.0</v>
+      </c>
+      <c r="R12" s="53"/>
+      <c r="S12" s="54">
+        <v>13.0</v>
+      </c>
+      <c r="T12" s="14"/>
+      <c r="U12" s="55">
+        <v>18.0</v>
+      </c>
+      <c r="V12" s="55">
+        <v>19.0</v>
+      </c>
+      <c r="W12" s="55">
+        <v>20.0</v>
+      </c>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="22"/>
+      <c r="AA12" s="27"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="12"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="5"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
-      <c r="AI12" s="5">
+      <c r="AI12" s="6">
         <v>10.0</v>
       </c>
       <c r="AJ12" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
-      <c r="AK12" s="2"/>
-      <c r="AL12" s="2"/>
+      <c r="AK12" s="17">
+        <v>42.0</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
@@ -1499,55 +1574,53 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="B13" s="56" t="s">
+        <v>20</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12">
-        <v>4.0</v>
-      </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="15">
-        <v>6.0</v>
-      </c>
-      <c r="N13" s="13"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="15">
-        <v>29.0</v>
-      </c>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="15">
-        <v>31.0</v>
-      </c>
-      <c r="AB13" s="13"/>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="17"/>
-      <c r="AE13" s="9"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="27"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="5"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
-      <c r="AI13" s="5">
+      <c r="AI13" s="6">
         <v>11.0</v>
       </c>
       <c r="AJ13" s="4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
-      <c r="AK13" s="2"/>
-      <c r="AL13" s="2"/>
+      <c r="AK13" s="17">
+        <v>43.0</v>
+      </c>
+      <c r="AL13" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
@@ -1559,55 +1632,65 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="5">
-        <v>3.0</v>
+      <c r="H14" s="2"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="57">
+        <v>8.0</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="21">
-        <v>5.0</v>
+      <c r="N14" s="19"/>
+      <c r="O14" s="13">
+        <v>9.0</v>
       </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="23">
-        <v>34.0</v>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="58">
+        <v>15.0</v>
       </c>
-      <c r="T14" s="16"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="22"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="22"/>
-      <c r="Y14" s="22"/>
-      <c r="Z14" s="22"/>
-      <c r="AA14" s="22"/>
-      <c r="AB14" s="22"/>
-      <c r="AC14" s="15">
-        <v>32.0</v>
+      <c r="U14" s="36">
+        <v>16.0</v>
       </c>
-      <c r="AD14" s="17"/>
-      <c r="AE14" s="9"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="59"/>
+      <c r="X14" s="60"/>
+      <c r="Y14" s="61"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="36">
+        <v>21.0</v>
+      </c>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="13">
+        <v>24.0</v>
+      </c>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="5"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
-      <c r="AI14" s="5">
+      <c r="AI14" s="6">
         <v>12.0</v>
       </c>
       <c r="AJ14" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
-      <c r="AK14" s="2"/>
-      <c r="AL14" s="2"/>
+      <c r="AK14" s="1">
+        <v>44.0</v>
+      </c>
+      <c r="AL14" s="62" t="s">
+        <v>25</v>
+      </c>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
@@ -1619,49 +1702,55 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="26"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="13">
+        <v>10.0</v>
+      </c>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="61"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="61"/>
       <c r="Z15" s="26"/>
       <c r="AA15" s="26"/>
-      <c r="AB15" s="16"/>
-      <c r="AC15" s="15">
-        <v>33.0</v>
-      </c>
-      <c r="AD15" s="17"/>
-      <c r="AE15" s="9"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="5"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
-      <c r="AI15" s="5">
+      <c r="AI15" s="6">
         <v>13.0</v>
       </c>
       <c r="AJ15" s="4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
-      <c r="AK15" s="2"/>
-      <c r="AL15" s="2"/>
+      <c r="AK15" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="AL15" s="63" t="s">
+        <v>28</v>
+      </c>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
@@ -1673,63 +1762,55 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="29">
-        <v>1.0</v>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="59"/>
+      <c r="V16" s="60"/>
+      <c r="W16" s="67"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="60"/>
+      <c r="Z16" s="60"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="13">
+        <v>25.0</v>
       </c>
-      <c r="I16" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="32">
-        <v>36.0</v>
-      </c>
-      <c r="M16" s="33">
-        <v>45.0</v>
-      </c>
-      <c r="N16" s="16"/>
-      <c r="O16" s="15">
-        <v>7.0</v>
-      </c>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="34">
-        <v>28.0</v>
-      </c>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="36">
-        <v>30.0</v>
-      </c>
-      <c r="X16" s="16"/>
-      <c r="Y16" s="34">
-        <v>23.0</v>
-      </c>
-      <c r="Z16" s="22"/>
-      <c r="AA16" s="27"/>
-      <c r="AB16" s="16"/>
-      <c r="AC16" s="37"/>
-      <c r="AD16" s="17"/>
-      <c r="AE16" s="9"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="5"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
-      <c r="AI16" s="5">
+      <c r="AI16" s="6">
         <v>14.0</v>
       </c>
       <c r="AJ16" s="4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
-      <c r="AK16" s="2"/>
-      <c r="AL16" s="2"/>
+      <c r="AK16" s="1">
+        <v>46.0</v>
+      </c>
+      <c r="AL16" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
@@ -1741,49 +1822,59 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="38">
-        <v>44.0</v>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="46">
+        <v>57.0</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="26"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="5"/>
       <c r="S17" s="26"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
-      <c r="V17" s="9"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="61"/>
+      <c r="V17" s="5"/>
       <c r="W17" s="26"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="27"/>
-      <c r="Z17" s="16"/>
-      <c r="AA17" s="27"/>
-      <c r="AB17" s="26"/>
-      <c r="AC17" s="26"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="68">
+        <v>27.0</v>
+      </c>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="13">
+        <v>26.0</v>
+      </c>
+      <c r="AD17" s="15"/>
+      <c r="AE17" s="5"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
-      <c r="AI17" s="5">
+      <c r="AI17" s="6">
         <v>15.0</v>
       </c>
       <c r="AJ17" s="4" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
-      <c r="AK17" s="2"/>
-      <c r="AL17" s="2"/>
+      <c r="AK17" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
@@ -1795,53 +1886,55 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="32">
-        <v>39.0</v>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="66"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="70"/>
+      <c r="Q18" s="13">
+        <v>12.0</v>
       </c>
-      <c r="K18" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="16"/>
-      <c r="M18" s="42">
-        <v>38.0</v>
-      </c>
-      <c r="N18" s="43"/>
-      <c r="O18" s="44"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="22"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="35"/>
-      <c r="Z18" s="16"/>
-      <c r="AA18" s="22"/>
-      <c r="AB18" s="22"/>
-      <c r="AC18" s="14"/>
-      <c r="AD18" s="17"/>
-      <c r="AE18" s="9"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="59"/>
+      <c r="T18" s="60"/>
+      <c r="U18" s="67"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="60"/>
+      <c r="Y18" s="60"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="60"/>
+      <c r="AB18" s="60"/>
+      <c r="AC18" s="67"/>
+      <c r="AD18" s="15"/>
+      <c r="AE18" s="5"/>
       <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
-      <c r="AI18" s="5">
+      <c r="AI18" s="6">
         <v>16.0</v>
       </c>
       <c r="AJ18" s="4" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
-      <c r="AK18" s="2"/>
-      <c r="AL18" s="2"/>
+      <c r="AK18" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="AL18" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" s="2"/>
@@ -1853,55 +1946,57 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="39" t="s">
-        <v>21</v>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="71">
+        <v>43.0</v>
       </c>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="46">
-        <v>18.0</v>
+      <c r="T19" s="5"/>
+      <c r="U19" s="72" t="s">
+        <v>39</v>
       </c>
-      <c r="T19" s="16"/>
-      <c r="U19" s="46">
-        <v>18.0</v>
-      </c>
-      <c r="V19" s="13"/>
-      <c r="W19" s="46">
-        <v>22.0</v>
-      </c>
-      <c r="X19" s="26"/>
-      <c r="Y19" s="26"/>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="26"/>
-      <c r="AB19" s="16"/>
-      <c r="AC19" s="14"/>
-      <c r="AD19" s="17"/>
-      <c r="AE19" s="9"/>
+      <c r="V19" s="43"/>
+      <c r="W19" s="43"/>
+      <c r="X19" s="43"/>
+      <c r="Y19" s="43"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
-      <c r="AI19" s="5">
+      <c r="AI19" s="6">
         <v>17.0</v>
       </c>
       <c r="AJ19" s="4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
-      <c r="AK19" s="2"/>
-      <c r="AL19" s="2"/>
+      <c r="AK19" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="AL19" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
@@ -1913,59 +2008,59 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="47">
-        <v>40.0</v>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="73">
+        <v>42.0</v>
       </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="51">
-        <v>11.0</v>
+      <c r="N20" s="40"/>
+      <c r="O20" s="6">
+        <v>14.0</v>
       </c>
-      <c r="R20" s="52"/>
-      <c r="S20" s="53">
-        <v>13.0</v>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="74"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="75"/>
+      <c r="V20" s="76"/>
+      <c r="W20" s="76"/>
+      <c r="X20" s="77">
+        <v>51.0</v>
       </c>
-      <c r="T20" s="16"/>
-      <c r="U20" s="54">
-        <v>18.0</v>
-      </c>
-      <c r="V20" s="54">
-        <v>19.0</v>
-      </c>
-      <c r="W20" s="54">
-        <v>20.0</v>
-      </c>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22"/>
-      <c r="Z20" s="22"/>
-      <c r="AA20" s="27"/>
-      <c r="AB20" s="16"/>
-      <c r="AC20" s="14"/>
-      <c r="AD20" s="17"/>
-      <c r="AE20" s="9"/>
+      <c r="Y20" s="78"/>
+      <c r="Z20" s="79"/>
+      <c r="AA20" s="80"/>
+      <c r="AB20" s="79"/>
+      <c r="AC20" s="81"/>
+      <c r="AD20" s="15"/>
+      <c r="AE20" s="5"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
-      <c r="AI20" s="5">
+      <c r="AI20" s="6">
         <v>18.0</v>
       </c>
       <c r="AJ20" s="4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
-      <c r="AK20" s="2"/>
-      <c r="AL20" s="2"/>
+      <c r="AK20" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="AL20" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
       <c r="AO20" s="2"/>
@@ -1977,129 +2072,121 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="B21" s="55" t="s">
-        <v>24</v>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="45"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="38">
+        <v>41.0</v>
+      </c>
       <c r="L21" s="43"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="26"/>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="16"/>
-      <c r="AA21" s="27"/>
-      <c r="AB21" s="16"/>
-      <c r="AC21" s="14"/>
-      <c r="AD21" s="17"/>
-      <c r="AE21" s="9"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="74"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="82"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="43"/>
+      <c r="Y21" s="83"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="82"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="84">
+        <v>52.0</v>
+      </c>
+      <c r="AD21" s="15"/>
+      <c r="AE21" s="5"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
-      <c r="AI21" s="5">
+      <c r="AI21" s="6">
         <v>19.0</v>
       </c>
       <c r="AJ21" s="4" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
-      <c r="AK21" s="2"/>
-      <c r="AL21" s="2"/>
-      <c r="AM21" s="2"/>
-      <c r="AN21" s="2"/>
-      <c r="AO21" s="2"/>
-      <c r="AP21" s="2"/>
-      <c r="AQ21" s="2"/>
-      <c r="AR21" s="2"/>
-      <c r="AS21" s="2"/>
+      <c r="AK21" s="1">
+        <v>51.0</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="AT21" s="2"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="39"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="85"/>
       <c r="L22" s="43"/>
-      <c r="M22" s="56">
-        <v>8.0</v>
+      <c r="M22" s="86"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="87"/>
+      <c r="R22" s="88"/>
+      <c r="S22" s="89">
+        <v>46.0</v>
       </c>
-      <c r="N22" s="19"/>
-      <c r="O22" s="15">
-        <v>9.0</v>
+      <c r="T22" s="5"/>
+      <c r="U22" s="84">
+        <v>48.0</v>
       </c>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="16"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="57">
-        <v>15.0</v>
+      <c r="V22" s="5"/>
+      <c r="W22" s="90">
+        <v>50.0</v>
       </c>
-      <c r="U22" s="36">
-        <v>16.0</v>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="91">
+        <v>53.0</v>
       </c>
-      <c r="V22" s="16"/>
-      <c r="W22" s="58"/>
-      <c r="X22" s="59"/>
-      <c r="Y22" s="60"/>
-      <c r="Z22" s="16"/>
-      <c r="AA22" s="36">
-        <v>21.0</v>
+      <c r="Z22" s="43"/>
+      <c r="AA22" s="83"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="92">
+        <v>54.0</v>
       </c>
-      <c r="AB22" s="16"/>
-      <c r="AC22" s="15">
-        <v>24.0</v>
-      </c>
-      <c r="AD22" s="17"/>
-      <c r="AE22" s="9"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="5"/>
       <c r="AF22" s="2"/>
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
-      <c r="AI22" s="5">
+      <c r="AI22" s="6">
         <v>20.0</v>
       </c>
-      <c r="AJ22" s="4" t="s">
-        <v>27</v>
+      <c r="AJ22" s="1" t="s">
+        <v>48</v>
       </c>
-      <c r="AK22" s="2"/>
-      <c r="AL22" s="2"/>
-      <c r="AM22" s="2"/>
-      <c r="AN22" s="2"/>
-      <c r="AO22" s="2"/>
-      <c r="AP22" s="2"/>
-      <c r="AQ22" s="2"/>
-      <c r="AR22" s="2"/>
-      <c r="AS22" s="2"/>
+      <c r="AK22" s="1">
+        <v>52.0</v>
+      </c>
+      <c r="AL22" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AT22" s="2"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="2"/>
-      <c r="B23" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2107,41 +2194,49 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="15">
-        <v>10.0</v>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="30">
+        <v>17.0</v>
       </c>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="13"/>
-      <c r="W23" s="60"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="60"/>
-      <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="16"/>
-      <c r="AC23" s="14"/>
-      <c r="AD23" s="17"/>
-      <c r="AE23" s="9"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="93"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="43"/>
+      <c r="U23" s="84"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="84">
+        <v>49.0</v>
+      </c>
+      <c r="X23" s="43"/>
+      <c r="Y23" s="94" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z23" s="43"/>
+      <c r="AA23" s="83"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
       <c r="AF23" s="2"/>
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
-      <c r="AI23" s="5">
+      <c r="AI23" s="6">
         <v>21.0</v>
       </c>
       <c r="AJ23" s="4" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
-      <c r="AK23" s="2"/>
-      <c r="AL23" s="2"/>
+      <c r="AK23" s="1">
+        <v>53.0</v>
+      </c>
+      <c r="AL23" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
@@ -2153,67 +2248,59 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="2"/>
-      <c r="B24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="2"/>
+      <c r="B24" s="4"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="61" t="s">
-        <v>19</v>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="87">
+        <v>47.0</v>
       </c>
-      <c r="L24" s="62"/>
-      <c r="M24" s="63"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="37"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="58"/>
-      <c r="V24" s="59"/>
-      <c r="W24" s="64"/>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="59"/>
-      <c r="Z24" s="59"/>
-      <c r="AA24" s="60"/>
-      <c r="AB24" s="16"/>
-      <c r="AC24" s="15">
-        <v>25.0</v>
+      <c r="P24" s="88"/>
+      <c r="Q24" s="95"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="96"/>
+      <c r="T24" s="76"/>
+      <c r="U24" s="97"/>
+      <c r="V24" s="76"/>
+      <c r="W24" s="98"/>
+      <c r="X24" s="43"/>
+      <c r="Y24" s="43"/>
+      <c r="Z24" s="43"/>
+      <c r="AA24" s="99"/>
+      <c r="AB24" s="100">
+        <v>56.0</v>
       </c>
-      <c r="AD24" s="17"/>
-      <c r="AE24" s="9"/>
+      <c r="AC24" s="101"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="5"/>
       <c r="AF24" s="2"/>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
-      <c r="AI24" s="5">
+      <c r="AI24" s="6">
         <v>22.0</v>
       </c>
       <c r="AJ24" s="4" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
-      <c r="AK24" s="2"/>
-      <c r="AL24" s="2"/>
-      <c r="AM24" s="2"/>
-      <c r="AN24" s="2"/>
-      <c r="AO24" s="2"/>
-      <c r="AP24" s="2"/>
-      <c r="AQ24" s="2"/>
-      <c r="AR24" s="2"/>
-      <c r="AS24" s="2"/>
+      <c r="AK24" s="1">
+        <v>54.0</v>
+      </c>
+      <c r="AL24" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="AT24" s="2"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="2"/>
-      <c r="B25" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="B25" s="4"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -2221,49 +2308,42 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="L25" s="43"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="60"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="13"/>
-      <c r="AA25" s="65">
-        <v>27.0</v>
-      </c>
-      <c r="AB25" s="13"/>
-      <c r="AC25" s="15">
-        <v>26.0</v>
-      </c>
-      <c r="AD25" s="17"/>
-      <c r="AE25" s="9"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="74"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="83"/>
+      <c r="T25" s="43"/>
+      <c r="U25" s="43"/>
+      <c r="V25" s="43"/>
+      <c r="W25" s="43"/>
+      <c r="X25" s="43"/>
+      <c r="Z25" s="43"/>
+      <c r="AA25" s="83"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
       <c r="AF25" s="2"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
-      <c r="AI25" s="5">
+      <c r="AI25" s="6">
         <v>23.0</v>
       </c>
       <c r="AJ25" s="4" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
-      <c r="AK25" s="2"/>
-      <c r="AL25" s="2"/>
-      <c r="AM25" s="2"/>
-      <c r="AN25" s="2"/>
-      <c r="AO25" s="2"/>
-      <c r="AP25" s="2"/>
+      <c r="AK25" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="AL25" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
       <c r="AS25" s="2"/>
@@ -2271,67 +2351,47 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="2"/>
-      <c r="B26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="66" t="s">
-        <v>19</v>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="102"/>
+      <c r="P26" s="79"/>
+      <c r="Q26" s="79"/>
+      <c r="R26" s="79"/>
+      <c r="S26" s="98"/>
+      <c r="T26" s="5"/>
+      <c r="Z26" s="43"/>
+      <c r="AA26" s="103"/>
+      <c r="AB26" s="79"/>
+      <c r="AC26" s="104">
+        <v>55.0</v>
       </c>
-      <c r="L26" s="62"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="63"/>
-      <c r="O26" s="63"/>
-      <c r="P26" s="67"/>
-      <c r="Q26" s="15">
-        <v>12.0</v>
-      </c>
-      <c r="R26" s="16"/>
-      <c r="S26" s="58"/>
-      <c r="T26" s="59"/>
-      <c r="U26" s="64"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="59"/>
-      <c r="X26" s="59"/>
-      <c r="Y26" s="59"/>
-      <c r="Z26" s="59"/>
-      <c r="AA26" s="59"/>
-      <c r="AB26" s="59"/>
-      <c r="AC26" s="64"/>
-      <c r="AD26" s="17"/>
-      <c r="AE26" s="9"/>
+      <c r="AD26" s="15"/>
+      <c r="AE26" s="5"/>
       <c r="AF26" s="2"/>
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
-      <c r="AI26" s="5">
+      <c r="AI26" s="6">
         <v>24.0</v>
       </c>
       <c r="AJ26" s="4" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
-      <c r="AK26" s="2"/>
-      <c r="AL26" s="2"/>
-      <c r="AM26" s="2"/>
-      <c r="AN26" s="2"/>
-      <c r="AO26" s="2"/>
-      <c r="AP26" s="2"/>
-      <c r="AQ26" s="2"/>
-      <c r="AR26" s="2"/>
-      <c r="AS26" s="2"/>
+      <c r="AK26" s="1">
+        <v>56.0</v>
+      </c>
+      <c r="AL26" s="105" t="s">
+        <v>58</v>
+      </c>
       <c r="AT26" s="2"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="2"/>
-      <c r="B27" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2339,43 +2399,47 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="68">
-        <v>43.0</v>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="106" t="s">
+        <v>59</v>
       </c>
-      <c r="T27" s="9"/>
-      <c r="U27" s="69" t="s">
-        <v>38</v>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="107"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="106" t="s">
+        <v>60</v>
       </c>
-      <c r="V27" s="43"/>
-      <c r="W27" s="43"/>
-      <c r="X27" s="43"/>
-      <c r="Y27" s="43"/>
-      <c r="Z27" s="9"/>
-      <c r="AA27" s="9"/>
-      <c r="AB27" s="9"/>
-      <c r="AC27" s="9"/>
-      <c r="AD27" s="9"/>
-      <c r="AE27" s="9"/>
+      <c r="AB27" s="15"/>
+      <c r="AC27" s="15"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
       <c r="AF27" s="2"/>
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
-      <c r="AI27" s="5">
+      <c r="AI27" s="6">
         <v>25.0</v>
       </c>
       <c r="AJ27" s="4" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
-      <c r="AK27" s="2"/>
-      <c r="AL27" s="2"/>
+      <c r="AK27" s="1">
+        <v>57.0</v>
+      </c>
+      <c r="AL27" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
       <c r="AO27" s="2"/>
@@ -2387,9 +2451,7 @@
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="A28" s="2"/>
-      <c r="B28" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2397,47 +2459,40 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="L28" s="62"/>
-      <c r="M28" s="70">
-        <v>42.0</v>
-      </c>
-      <c r="N28" s="40"/>
-      <c r="O28" s="5">
-        <v>14.0</v>
-      </c>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="71"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="72"/>
-      <c r="V28" s="73"/>
-      <c r="W28" s="73"/>
-      <c r="X28" s="74">
-        <v>51.0</v>
-      </c>
-      <c r="Y28" s="75"/>
-      <c r="Z28" s="76"/>
-      <c r="AA28" s="77"/>
-      <c r="AB28" s="76"/>
-      <c r="AC28" s="78"/>
-      <c r="AD28" s="17"/>
-      <c r="AE28" s="9"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="43"/>
+      <c r="V28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="43"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
-      <c r="AI28" s="5">
+      <c r="AI28" s="6">
         <v>26.0</v>
       </c>
-      <c r="AJ28" s="79" t="s">
-        <v>41</v>
+      <c r="AJ28" s="8" t="s">
+        <v>63</v>
       </c>
-      <c r="AK28" s="2"/>
-      <c r="AL28" s="2"/>
+      <c r="AK28" s="1">
+        <v>58.0</v>
+      </c>
+      <c r="AL28" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="AM28" s="2"/>
       <c r="AN28" s="2"/>
       <c r="AO28" s="2"/>
@@ -2449,9 +2504,7 @@
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="A29" s="2"/>
-      <c r="B29" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2459,40 +2512,33 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="38">
-        <v>41.0</v>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="4" t="s">
+        <v>65</v>
       </c>
-      <c r="L29" s="43"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="71"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="80"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="43"/>
-      <c r="Y29" s="81"/>
-      <c r="Z29" s="9"/>
-      <c r="AA29" s="80"/>
-      <c r="AB29" s="9"/>
-      <c r="AC29" s="82">
-        <v>52.0</v>
-      </c>
-      <c r="AD29" s="17"/>
-      <c r="AE29" s="9"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
       <c r="AH29" s="2"/>
-      <c r="AI29" s="5">
+      <c r="AI29" s="6">
         <v>27.0</v>
       </c>
       <c r="AJ29" s="4" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="AK29" s="2"/>
       <c r="AL29" s="2"/>
@@ -2508,56 +2554,35 @@
     <row r="30" ht="13.5" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="83"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="84"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="37"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="85"/>
-      <c r="R30" s="86"/>
-      <c r="S30" s="87">
-        <v>46.0</v>
+      <c r="D30" s="108" t="s">
+        <v>50</v>
       </c>
-      <c r="T30" s="9"/>
-      <c r="U30" s="82">
-        <v>48.0</v>
+      <c r="E30" s="108" t="s">
+        <v>67</v>
       </c>
-      <c r="V30" s="9"/>
-      <c r="W30" s="88">
-        <v>50.0</v>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="59"/>
+      <c r="X30" s="4" t="s">
+        <v>68</v>
       </c>
-      <c r="X30" s="43"/>
-      <c r="Y30" s="89">
-        <v>53.0</v>
-      </c>
-      <c r="Z30" s="43"/>
-      <c r="AA30" s="81"/>
-      <c r="AB30" s="9"/>
-      <c r="AC30" s="90">
-        <v>54.0</v>
-      </c>
-      <c r="AD30" s="17"/>
-      <c r="AE30" s="9"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
       <c r="AH30" s="2"/>
-      <c r="AI30" s="5">
+      <c r="AI30" s="6">
         <v>28.0</v>
       </c>
       <c r="AJ30" s="4" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
-      <c r="AK30" s="2"/>
-      <c r="AL30" s="2"/>
       <c r="AM30" s="2"/>
       <c r="AN30" s="2"/>
       <c r="AO30" s="2"/>
@@ -2570,52 +2595,28 @@
     <row r="31" ht="13.5" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="30">
-        <v>17.0</v>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="109"/>
+      <c r="X31" s="4" t="s">
+        <v>70</v>
       </c>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="91"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="43"/>
-      <c r="T31" s="43"/>
-      <c r="U31" s="82"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="82">
-        <v>49.0</v>
-      </c>
-      <c r="X31" s="43"/>
-      <c r="Y31" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z31" s="43"/>
-      <c r="AA31" s="81"/>
-      <c r="AB31" s="9"/>
-      <c r="AC31" s="9"/>
-      <c r="AD31" s="9"/>
-      <c r="AE31" s="9"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="2"/>
+      <c r="AD31" s="2"/>
+      <c r="AE31" s="2"/>
       <c r="AF31" s="2"/>
       <c r="AG31" s="2"/>
       <c r="AH31" s="2"/>
-      <c r="AI31" s="5">
+      <c r="AI31" s="6">
         <v>29.0</v>
       </c>
       <c r="AJ31" s="4" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
-      <c r="AK31" s="2"/>
-      <c r="AL31" s="2"/>
       <c r="AM31" s="2"/>
       <c r="AN31" s="2"/>
       <c r="AO31" s="2"/>
@@ -2627,47 +2628,42 @@
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="2"/>
-      <c r="B32" s="4"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="85">
-        <v>47.0</v>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="24"/>
+      <c r="X32" s="4" t="s">
+        <v>72</v>
       </c>
-      <c r="P32" s="86"/>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="94"/>
-      <c r="T32" s="73"/>
-      <c r="U32" s="95"/>
-      <c r="V32" s="73"/>
-      <c r="W32" s="96"/>
-      <c r="X32" s="43"/>
-      <c r="Y32" s="43"/>
-      <c r="Z32" s="43"/>
-      <c r="AA32" s="97"/>
-      <c r="AB32" s="98">
-        <v>56.0</v>
-      </c>
-      <c r="AC32" s="99"/>
-      <c r="AD32" s="17"/>
-      <c r="AE32" s="9"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
       <c r="AF32" s="2"/>
       <c r="AG32" s="2"/>
       <c r="AH32" s="2"/>
-      <c r="AI32" s="5">
+      <c r="AI32" s="6">
         <v>30.0</v>
       </c>
       <c r="AJ32" s="4" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="AK32" s="2"/>
       <c r="AL32" s="2"/>
@@ -2682,7 +2678,7 @@
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -2690,35 +2686,37 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="71"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="81"/>
-      <c r="T33" s="43"/>
-      <c r="U33" s="43"/>
-      <c r="V33" s="43"/>
-      <c r="W33" s="43"/>
-      <c r="X33" s="43"/>
-      <c r="Z33" s="43"/>
-      <c r="AA33" s="81"/>
-      <c r="AB33" s="9"/>
-      <c r="AC33" s="9"/>
-      <c r="AD33" s="9"/>
-      <c r="AE33" s="9"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="110"/>
+      <c r="X33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
       <c r="AF33" s="2"/>
       <c r="AG33" s="2"/>
       <c r="AH33" s="2"/>
-      <c r="AI33" s="5">
+      <c r="AI33" s="6">
         <v>31.0</v>
       </c>
       <c r="AJ33" s="4" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="AK33" s="2"/>
       <c r="AL33" s="2"/>
@@ -2733,35 +2731,45 @@
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="100"/>
-      <c r="P34" s="76"/>
-      <c r="Q34" s="76"/>
-      <c r="R34" s="76"/>
-      <c r="S34" s="96"/>
-      <c r="T34" s="9"/>
-      <c r="Z34" s="43"/>
-      <c r="AA34" s="101"/>
-      <c r="AB34" s="76"/>
-      <c r="AC34" s="102">
-        <v>55.0</v>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="111"/>
+      <c r="X34" s="1" t="s">
+        <v>76</v>
       </c>
-      <c r="AD34" s="17"/>
-      <c r="AE34" s="9"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
-      <c r="AI34" s="5">
+      <c r="AI34" s="6">
         <v>32.0</v>
       </c>
       <c r="AJ34" s="4" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="AK34" s="2"/>
       <c r="AL34" s="2"/>
@@ -2775,54 +2783,11 @@
       <c r="AT34" s="2"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>19</v>
+      <c r="S35" s="112" t="s">
+        <v>78</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="17"/>
-      <c r="S35" s="104"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
-      <c r="X35" s="2"/>
-      <c r="Y35" s="2"/>
-      <c r="Z35" s="9"/>
-      <c r="AA35" s="103" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB35" s="17"/>
-      <c r="AC35" s="17"/>
-      <c r="AD35" s="9"/>
-      <c r="AE35" s="9"/>
-      <c r="AF35" s="2"/>
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
-      <c r="AI35" s="5">
-        <v>33.0</v>
-      </c>
-      <c r="AJ35" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="AK35" s="2"/>
       <c r="AL35" s="2"/>
       <c r="AM35" s="2"/>
@@ -2835,47 +2800,11 @@
       <c r="AT35" s="2"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>33</v>
+      <c r="A36" s="1" t="s">
+        <v>79</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="43"/>
-      <c r="T36" s="43"/>
-      <c r="V36" s="2"/>
-      <c r="Y36" s="2"/>
-      <c r="Z36" s="9"/>
-      <c r="AA36" s="9"/>
-      <c r="AB36" s="9"/>
-      <c r="AC36" s="43"/>
-      <c r="AD36" s="9"/>
-      <c r="AE36" s="2"/>
-      <c r="AF36" s="2"/>
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
-      <c r="AI36" s="5">
-        <v>34.0</v>
-      </c>
-      <c r="AJ36" s="79" t="s">
-        <v>55</v>
-      </c>
       <c r="AK36" s="2"/>
       <c r="AL36" s="2"/>
       <c r="AM36" s="2"/>
@@ -2887,47 +2816,13 @@
       <c r="AT36" s="2"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
-        <v>21</v>
+      <c r="A37" s="1" t="s">
+        <v>80</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="V37" s="2"/>
-      <c r="W37" s="17"/>
-      <c r="X37" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y37" s="2"/>
-      <c r="Z37" s="2"/>
-      <c r="AA37" s="2"/>
-      <c r="AB37" s="2"/>
-      <c r="AD37" s="2"/>
-      <c r="AE37" s="2"/>
-      <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
-      <c r="AI37" s="105">
-        <v>35.0</v>
-      </c>
-      <c r="AJ37" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="AI37" s="17"/>
+      <c r="AJ37" s="1"/>
       <c r="AK37" s="2"/>
       <c r="AL37" s="2"/>
       <c r="AM37" s="2"/>
@@ -2940,37 +2835,13 @@
       <c r="AT37" s="2"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="D38" s="106" t="s">
-        <v>45</v>
+      <c r="A38" s="2" t="s">
+        <v>81</v>
       </c>
-      <c r="E38" s="106" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="V38" s="2"/>
-      <c r="W38" s="58"/>
-      <c r="X38" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y38" s="2"/>
-      <c r="Z38" s="2"/>
-      <c r="AA38" s="2"/>
-      <c r="AB38" s="2"/>
-      <c r="AC38" s="2"/>
-      <c r="AD38" s="2"/>
-      <c r="AE38" s="2"/>
-      <c r="AF38" s="2"/>
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
-      <c r="AI38" s="105">
-        <v>36.0</v>
-      </c>
-      <c r="AJ38" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="AI38" s="17"/>
+      <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
       <c r="AL38" s="2"/>
       <c r="AM38" s="2"/>
@@ -2983,30 +2854,13 @@
       <c r="AT38" s="2"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="107"/>
-      <c r="X39" s="4" t="s">
-        <v>62</v>
+      <c r="A39" s="2" t="s">
+        <v>82</v>
       </c>
-      <c r="Y39" s="2"/>
-      <c r="Z39" s="2"/>
-      <c r="AA39" s="2"/>
-      <c r="AB39" s="2"/>
-      <c r="AD39" s="2"/>
-      <c r="AE39" s="2"/>
-      <c r="AF39" s="2"/>
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
-      <c r="AI39" s="105">
-        <v>37.0</v>
-      </c>
-      <c r="AJ39" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="AI39" s="17"/>
+      <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
       <c r="AL39" s="1"/>
       <c r="AM39" s="2"/>
@@ -3019,44 +2873,13 @@
       <c r="AT39" s="2"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="V40" s="2"/>
-      <c r="W40" s="24"/>
-      <c r="X40" s="4" t="s">
-        <v>64</v>
+      <c r="A40" s="2" t="s">
+        <v>83</v>
       </c>
-      <c r="Y40" s="2"/>
-      <c r="Z40" s="2"/>
-      <c r="AA40" s="2"/>
-      <c r="AB40" s="2"/>
-      <c r="AD40" s="2"/>
-      <c r="AE40" s="2"/>
-      <c r="AF40" s="2"/>
       <c r="AG40" s="2"/>
       <c r="AH40" s="2"/>
-      <c r="AI40" s="105">
-        <v>38.0</v>
-      </c>
-      <c r="AJ40" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="AI40" s="17"/>
+      <c r="AJ40" s="2"/>
       <c r="AK40" s="2"/>
       <c r="AL40" s="2"/>
       <c r="AM40" s="2"/>
@@ -3069,47 +2892,13 @@
       <c r="AT40" s="2"/>
     </row>
     <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="2"/>
-      <c r="T41" s="2"/>
-      <c r="U41" s="2"/>
-      <c r="V41" s="2"/>
-      <c r="W41" s="108"/>
-      <c r="X41" s="2" t="s">
-        <v>66</v>
+      <c r="A41" s="1" t="s">
+        <v>84</v>
       </c>
-      <c r="Y41" s="2"/>
-      <c r="Z41" s="2"/>
-      <c r="AA41" s="2"/>
-      <c r="AB41" s="2"/>
-      <c r="AC41" s="2"/>
-      <c r="AD41" s="2"/>
-      <c r="AE41" s="2"/>
-      <c r="AF41" s="2"/>
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
-      <c r="AI41" s="105">
-        <v>39.0</v>
-      </c>
-      <c r="AJ41" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="AI41" s="17"/>
+      <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
       <c r="AL41" s="2"/>
       <c r="AM41" s="2"/>
@@ -3122,47 +2911,13 @@
       <c r="AT41" s="2"/>
     </row>
     <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="T42" s="2"/>
-      <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
-      <c r="W42" s="109"/>
-      <c r="X42" s="1" t="s">
-        <v>68</v>
+      <c r="A42" s="1" t="s">
+        <v>85</v>
       </c>
-      <c r="Y42" s="2"/>
-      <c r="Z42" s="2"/>
-      <c r="AA42" s="2"/>
-      <c r="AB42" s="2"/>
-      <c r="AC42" s="2"/>
-      <c r="AD42" s="2"/>
-      <c r="AE42" s="2"/>
-      <c r="AF42" s="2"/>
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
-      <c r="AI42" s="105">
-        <v>40.0</v>
-      </c>
-      <c r="AJ42" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="AI42" s="17"/>
+      <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
       <c r="AL42" s="2"/>
       <c r="AM42" s="2"/>
@@ -3192,9 +2947,6 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
-      <c r="S43" s="110" t="s">
-        <v>70</v>
-      </c>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
@@ -3210,12 +2962,8 @@
       <c r="AF43" s="2"/>
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
-      <c r="AI43" s="105">
-        <v>41.0</v>
-      </c>
-      <c r="AJ43" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="AI43" s="17"/>
+      <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
       <c r="AL43" s="2"/>
       <c r="AM43" s="2"/>
@@ -3228,15 +2976,14 @@
       <c r="AT43" s="2"/>
     </row>
     <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="2" t="s">
-        <v>72</v>
+      <c r="B44" s="113"/>
+      <c r="C44" s="114" t="s">
+        <v>86</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="D44" s="113"/>
+      <c r="E44" s="113"/>
+      <c r="F44" s="113"/>
+      <c r="G44" s="113"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -3264,12 +3011,8 @@
       <c r="AF44" s="2"/>
       <c r="AG44" s="2"/>
       <c r="AH44" s="2"/>
-      <c r="AI44" s="105">
-        <v>42.0</v>
-      </c>
-      <c r="AJ44" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="AI44" s="17"/>
+      <c r="AJ44" s="1"/>
       <c r="AK44" s="2"/>
       <c r="AL44" s="2"/>
       <c r="AM44" s="2"/>
@@ -3282,15 +3025,14 @@
       <c r="AT44" s="2"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="2" t="s">
-        <v>74</v>
+      <c r="B45" s="113"/>
+      <c r="C45" s="114" t="s">
+        <v>87</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="D45" s="113"/>
+      <c r="E45" s="113"/>
+      <c r="F45" s="113"/>
+      <c r="G45" s="113"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -3318,12 +3060,8 @@
       <c r="AF45" s="2"/>
       <c r="AG45" s="2"/>
       <c r="AH45" s="2"/>
-      <c r="AI45" s="105">
-        <v>43.0</v>
-      </c>
-      <c r="AJ45" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="AI45" s="17"/>
+      <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
       <c r="AL45" s="2"/>
       <c r="AM45" s="2"/>
@@ -3336,9 +3074,6 @@
       <c r="AT45" s="2"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -3372,12 +3107,8 @@
       <c r="AF46" s="2"/>
       <c r="AG46" s="2"/>
       <c r="AH46" s="2"/>
-      <c r="AI46" s="1">
-        <v>44.0</v>
-      </c>
-      <c r="AJ46" s="111" t="s">
-        <v>77</v>
-      </c>
+      <c r="AI46" s="1"/>
+      <c r="AJ46" s="62"/>
       <c r="AK46" s="2"/>
       <c r="AL46" s="2"/>
       <c r="AM46" s="2"/>
@@ -3390,9 +3121,6 @@
       <c r="AT46" s="2"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -3426,10 +3154,8 @@
       <c r="AF47" s="2"/>
       <c r="AG47" s="2"/>
       <c r="AH47" s="2"/>
-      <c r="AI47" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ47" s="2"/>
+      <c r="AI47" s="1"/>
+      <c r="AJ47" s="1"/>
       <c r="AK47" s="2"/>
       <c r="AL47" s="2"/>
       <c r="AM47" s="2"/>
@@ -3442,9 +3168,6 @@
       <c r="AT47" s="2"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
-      <c r="A48" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -3478,12 +3201,8 @@
       <c r="AF48" s="2"/>
       <c r="AG48" s="2"/>
       <c r="AH48" s="2"/>
-      <c r="AI48" s="1">
-        <v>46.0</v>
-      </c>
-      <c r="AJ48" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="AI48" s="1"/>
+      <c r="AJ48" s="1"/>
       <c r="AK48" s="2"/>
       <c r="AL48" s="2"/>
       <c r="AM48" s="2"/>
@@ -3496,9 +3215,6 @@
       <c r="AT48" s="2"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -3532,12 +3248,8 @@
       <c r="AF49" s="2"/>
       <c r="AG49" s="2"/>
       <c r="AH49" s="2"/>
-      <c r="AI49" s="1">
-        <v>47.0</v>
-      </c>
-      <c r="AJ49" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="AI49" s="1"/>
+      <c r="AJ49" s="1"/>
       <c r="AK49" s="2"/>
       <c r="AL49" s="2"/>
       <c r="AM49" s="2"/>
@@ -3550,7 +3262,6 @@
       <c r="AT49" s="2"/>
     </row>
     <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -3584,12 +3295,8 @@
       <c r="AF50" s="2"/>
       <c r="AG50" s="2"/>
       <c r="AH50" s="2"/>
-      <c r="AI50" s="1">
-        <v>48.0</v>
-      </c>
-      <c r="AJ50" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="AI50" s="1"/>
+      <c r="AJ50" s="1"/>
       <c r="AK50" s="2"/>
       <c r="AL50" s="2"/>
       <c r="AM50" s="2"/>
@@ -3636,12 +3343,8 @@
       <c r="AF51" s="2"/>
       <c r="AG51" s="2"/>
       <c r="AH51" s="2"/>
-      <c r="AI51" s="1">
-        <v>49.0</v>
-      </c>
-      <c r="AJ51" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="AI51" s="1"/>
+      <c r="AJ51" s="1"/>
       <c r="AK51" s="2"/>
       <c r="AL51" s="2"/>
       <c r="AM51" s="2"/>
@@ -3688,12 +3391,8 @@
       <c r="AF52" s="2"/>
       <c r="AG52" s="2"/>
       <c r="AH52" s="2"/>
-      <c r="AI52" s="1">
-        <v>50.0</v>
-      </c>
-      <c r="AJ52" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="AI52" s="1"/>
+      <c r="AJ52" s="1"/>
       <c r="AK52" s="2"/>
       <c r="AL52" s="2"/>
       <c r="AM52" s="2"/>
@@ -3740,24 +3439,14 @@
       <c r="AF53" s="2"/>
       <c r="AG53" s="2"/>
       <c r="AH53" s="2"/>
-      <c r="AI53" s="1">
-        <v>51.0</v>
-      </c>
-      <c r="AJ53" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="AI53" s="1"/>
+      <c r="AJ53" s="1"/>
       <c r="AR53" s="2"/>
       <c r="AS53" s="2"/>
       <c r="AT53" s="2"/>
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -3785,24 +3474,14 @@
       <c r="AF54" s="2"/>
       <c r="AG54" s="2"/>
       <c r="AH54" s="2"/>
-      <c r="AI54" s="1">
-        <v>52.0</v>
-      </c>
-      <c r="AJ54" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="AI54" s="1"/>
+      <c r="AJ54" s="1"/>
       <c r="AR54" s="2"/>
       <c r="AS54" s="2"/>
       <c r="AT54" s="2"/>
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -3830,12 +3509,8 @@
       <c r="AF55" s="2"/>
       <c r="AG55" s="2"/>
       <c r="AH55" s="2"/>
-      <c r="AI55" s="1">
-        <v>53.0</v>
-      </c>
-      <c r="AJ55" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="AI55" s="1"/>
+      <c r="AJ55" s="1"/>
       <c r="AK55" s="2"/>
       <c r="AL55" s="2"/>
       <c r="AM55" s="2"/>
@@ -3882,12 +3557,8 @@
       <c r="AF56" s="2"/>
       <c r="AG56" s="2"/>
       <c r="AH56" s="2"/>
-      <c r="AI56" s="1">
-        <v>54.0</v>
-      </c>
-      <c r="AJ56" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="AI56" s="1"/>
+      <c r="AJ56" s="1"/>
       <c r="AR56" s="2"/>
       <c r="AS56" s="2"/>
       <c r="AT56" s="2"/>
@@ -3927,12 +3598,8 @@
       <c r="AF57" s="2"/>
       <c r="AG57" s="2"/>
       <c r="AH57" s="2"/>
-      <c r="AI57" s="1">
-        <v>55.0</v>
-      </c>
-      <c r="AJ57" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="AI57" s="1"/>
+      <c r="AJ57" s="1"/>
       <c r="AO57" s="2"/>
       <c r="AP57" s="2"/>
       <c r="AQ57" s="2"/>
@@ -3975,12 +3642,8 @@
       <c r="AF58" s="2"/>
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
-      <c r="AI58" s="1">
-        <v>56.0</v>
-      </c>
-      <c r="AJ58" s="112" t="s">
-        <v>92</v>
-      </c>
+      <c r="AI58" s="1"/>
+      <c r="AJ58" s="105"/>
       <c r="AR58" s="2"/>
       <c r="AS58" s="2"/>
       <c r="AT58" s="2"/>
@@ -4020,8 +3683,8 @@
       <c r="AF59" s="2"/>
       <c r="AG59" s="2"/>
       <c r="AH59" s="2"/>
-      <c r="AI59" s="2"/>
-      <c r="AJ59" s="2"/>
+      <c r="AI59" s="1"/>
+      <c r="AJ59" s="1"/>
       <c r="AK59" s="2"/>
       <c r="AL59" s="2"/>
       <c r="AM59" s="2"/>
@@ -4068,7 +3731,7 @@
       <c r="AF60" s="2"/>
       <c r="AG60" s="2"/>
       <c r="AH60" s="2"/>
-      <c r="AI60" s="2"/>
+      <c r="AI60" s="1"/>
       <c r="AJ60" s="2"/>
       <c r="AK60" s="2"/>
       <c r="AL60" s="2"/>
@@ -49298,12 +48961,17 @@
       <c r="AT1002" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="AL24:AS24"/>
+    <mergeCell ref="AL25:AP25"/>
+    <mergeCell ref="AL21:AS21"/>
+    <mergeCell ref="AL22:AS22"/>
     <mergeCell ref="AJ53:AQ53"/>
     <mergeCell ref="AJ54:AQ54"/>
     <mergeCell ref="AJ56:AQ56"/>
     <mergeCell ref="AJ57:AN57"/>
     <mergeCell ref="AJ58:AQ58"/>
+    <mergeCell ref="AL26:AS26"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add kastle_38, _40, and _42 that will put a krieger clone at those locations to push the red button which will release the octopus
</commit_message>
<xml_diff>
--- a/Krieger Kastle.xlsx
+++ b/Krieger Kastle.xlsx
@@ -11,13 +11,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
   <si>
     <t>
 </t>
   </si>
   <si>
+    <t>META GAME</t>
+  </si>
+  <si>
     <t>legend</t>
+  </si>
+  <si>
+    <t>Type 'quit'</t>
   </si>
   <si>
     <t>start, stick</t>
@@ -134,7 +140,7 @@
     <t>43 Requires Bomb to go south</t>
   </si>
   <si>
-    <t>Missing 2112 album</t>
+    <t>Missing 2112 album, moving bookshelf</t>
   </si>
   <si>
     <t>candy bar wrapper, modern art</t>
@@ -179,6 +185,9 @@
     <t>Spatula, Little Hat</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>cesta</t>
   </si>
   <si>
@@ -215,6 +224,9 @@
     <t>Other Other Barry, need chainsaw or other</t>
   </si>
   <si>
+    <t>Rush concept album</t>
+  </si>
+  <si>
     <t>Big Robot</t>
   </si>
   <si>
@@ -224,10 +236,19 @@
     <t>gator tooth</t>
   </si>
   <si>
+    <t>clicker (can't pick up)</t>
+  </si>
+  <si>
+    <t>Mitsuko, gives you spoon and wants kidneys in return</t>
+  </si>
+  <si>
     <t>Van</t>
   </si>
   <si>
     <t>bowling ball</t>
+  </si>
+  <si>
+    <t>"ethereal glow of finality"</t>
   </si>
   <si>
     <t>Jungle</t>
@@ -254,7 +275,7 @@
     <t>you can construct a dry ice bomb with a bottle, water, dry ice, and bottlecap (fill bottle with water from pond at 16, 'use ice on beer', 'use cap on bomb', RUN)</t>
   </si>
   <si>
-    <t>having three people hold down all three console buttons at 38/40/42 releases a murderous octopus from the cryo chamber ('press button')</t>
+    <t>having three people hold down the console buttons at 38/40/42 releases a murderous octopus from the cryo chamber ('push button'), it heads for the giant robot at R</t>
   </si>
   <si>
     <t>the lab door on the west wall of 12 requires keycard from 43 to open</t>
@@ -272,10 +293,10 @@
     <t>43 requires dry ice bomb to get past, cave will cave in and kill you after a few seconds if you don't rush back by</t>
   </si>
   <si>
-    <t>META GAME</t>
+    <t>To get past the giant robot, you must let the octopus out, and rush past the octopus fighting the giant robot as they fight (only a few second window)</t>
   </si>
   <si>
-    <t>Type 'quit'</t>
+    <t>Missing rush album is at 59. Bring it back past the giant robot, collapsing cave, and cave door (good luck) and place it at 17 to reveal a new path</t>
   </si>
 </sst>
 </file>
@@ -309,12 +330,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -376,20 +403,8 @@
         <bgColor rgb="FFE69138"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB45F06"/>
-        <bgColor rgb="FFB45F06"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -421,6 +436,14 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+    </border>
+    <border>
+      <left style="dashed">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
     </border>
     <border>
       <left style="thin">
@@ -493,6 +516,38 @@
       </bottom>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -524,11 +579,23 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="123">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -538,31 +605,37 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -571,19 +644,19 @@
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -592,28 +665,31 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -622,226 +698,241 @@
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="5" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="5" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="6" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="7" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="8" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
     </xf>
     <xf borderId="3" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="8" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="2" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="9" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="1" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="3" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="1" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="5" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="10" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="13" fillId="11" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="7" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="6" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="7" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="7" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="5" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="6" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="16" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="8" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="9" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="8" fillId="12" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="3" fillId="12" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="17" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="4" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="5" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="12" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="7" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="8" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="7" fillId="11" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="11" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="13" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="10" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -870,7 +961,7 @@
     <col customWidth="1" min="39" max="46" width="3.29"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1">
+    <row r="1" ht="19.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,13 +1011,15 @@
       <c r="AS1" s="2"/>
       <c r="AT1" s="2"/>
     </row>
-    <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -955,8 +1048,8 @@
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
-      <c r="AI2" s="3" t="s">
-        <v>1</v>
+      <c r="AI2" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
@@ -965,57 +1058,59 @@
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
       <c r="AP2" s="2"/>
-      <c r="AQ2" s="4"/>
-      <c r="AR2" s="4"/>
+      <c r="AQ2" s="6"/>
+      <c r="AR2" s="6"/>
       <c r="AS2" s="2"/>
       <c r="AT2" s="2"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="2"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
-      <c r="AI3" s="6">
+      <c r="AI3" s="8">
         <v>1.0</v>
       </c>
-      <c r="AJ3" s="4" t="s">
-        <v>2</v>
+      <c r="AJ3" s="6" t="s">
+        <v>4</v>
       </c>
-      <c r="AK3" s="6">
+      <c r="AK3" s="8">
         <v>33.0</v>
       </c>
-      <c r="AL3" s="4" t="s">
-        <v>3</v>
+      <c r="AL3" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="AT3" s="2"/>
     </row>
@@ -1027,44 +1122,44 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
-      <c r="AI4" s="6">
+      <c r="AI4" s="8">
         <v>2.0</v>
       </c>
-      <c r="AJ4" s="4" t="s">
-        <v>4</v>
+      <c r="AJ4" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="AK4" s="6">
+      <c r="AK4" s="8">
         <v>34.0</v>
       </c>
-      <c r="AL4" s="8" t="s">
-        <v>5</v>
+      <c r="AL4" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="AT4" s="2"/>
     </row>
@@ -1076,48 +1171,48 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10">
+      <c r="H5" s="11"/>
+      <c r="I5" s="12">
         <v>4.0</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="13">
+      <c r="J5" s="13"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="15">
         <v>6.0</v>
       </c>
-      <c r="N5" s="11"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="13">
+      <c r="N5" s="13"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="15">
         <v>29.0</v>
       </c>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="13">
+      <c r="X5" s="13"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="15">
         <v>31.0</v>
       </c>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="5"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="7"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
-      <c r="AI5" s="6">
+      <c r="AI5" s="8">
         <v>3.0</v>
       </c>
-      <c r="AJ5" s="16" t="s">
-        <v>6</v>
+      <c r="AJ5" s="18" t="s">
+        <v>8</v>
       </c>
-      <c r="AK5" s="17">
+      <c r="AK5" s="19">
         <v>35.0</v>
       </c>
       <c r="AL5" s="1"/>
@@ -1138,52 +1233,52 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="6">
+      <c r="H6" s="20"/>
+      <c r="I6" s="8">
         <v>3.0</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="21">
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="23">
         <v>5.0</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="23">
+      <c r="O6" s="24"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="26">
         <v>34.0</v>
       </c>
-      <c r="T6" s="14"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="13">
+      <c r="T6" s="16"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="15">
         <v>32.0</v>
       </c>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="5"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="7"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
-      <c r="AI6" s="6">
+      <c r="AI6" s="8">
         <v>4.0</v>
       </c>
-      <c r="AJ6" s="4" t="s">
-        <v>7</v>
+      <c r="AJ6" s="6" t="s">
+        <v>9</v>
       </c>
-      <c r="AK6" s="17">
+      <c r="AK6" s="19">
         <v>36.0</v>
       </c>
       <c r="AL6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
@@ -1200,44 +1295,44 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="27"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="13">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="15">
         <v>33.0</v>
       </c>
-      <c r="AD7" s="15"/>
-      <c r="AE7" s="5"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="7"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
-      <c r="AI7" s="6">
+      <c r="AI7" s="8">
         <v>5.0</v>
       </c>
-      <c r="AJ7" s="4" t="s">
-        <v>9</v>
+      <c r="AJ7" s="6" t="s">
+        <v>11</v>
       </c>
-      <c r="AK7" s="17">
+      <c r="AK7" s="19">
         <v>37.0</v>
       </c>
       <c r="AL7" s="2"/>
@@ -1256,62 +1351,62 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29">
+      <c r="F8" s="7"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32">
         <v>1.0</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="33">
         <v>2.0</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="32">
+      <c r="J8" s="7"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="35">
         <v>36.0</v>
       </c>
-      <c r="M8" s="33">
+      <c r="M8" s="36">
         <v>45.0</v>
       </c>
-      <c r="N8" s="14"/>
-      <c r="O8" s="13">
+      <c r="N8" s="16"/>
+      <c r="O8" s="15">
         <v>7.0</v>
       </c>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="34">
+      <c r="P8" s="16"/>
+      <c r="Q8" s="37">
         <v>28.0</v>
       </c>
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="36">
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="39">
         <v>30.0</v>
       </c>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="34">
+      <c r="X8" s="16"/>
+      <c r="Y8" s="37">
         <v>23.0</v>
       </c>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="27"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="37"/>
-      <c r="AD8" s="15"/>
-      <c r="AE8" s="5"/>
+      <c r="Z8" s="25"/>
+      <c r="AA8" s="30"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="40"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="7"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
-      <c r="AI8" s="6">
+      <c r="AI8" s="8">
         <v>6.0</v>
       </c>
-      <c r="AJ8" s="4" t="s">
-        <v>10</v>
+      <c r="AJ8" s="6" t="s">
+        <v>12</v>
       </c>
-      <c r="AK8" s="17">
+      <c r="AK8" s="19">
         <v>38.0</v>
       </c>
       <c r="AL8" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
@@ -1328,48 +1423,48 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="38">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="41">
         <v>44.0</v>
       </c>
-      <c r="L9" s="14"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="27"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="5"/>
-      <c r="AE9" s="5"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="30"/>
+      <c r="AB9" s="29"/>
+      <c r="AC9" s="29"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
-      <c r="AI9" s="6">
+      <c r="AI9" s="8">
         <v>7.0</v>
       </c>
-      <c r="AJ9" s="4" t="s">
-        <v>12</v>
+      <c r="AJ9" s="6" t="s">
+        <v>14</v>
       </c>
-      <c r="AK9" s="17">
+      <c r="AK9" s="19">
         <v>39.0</v>
       </c>
       <c r="AL9" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
@@ -1383,53 +1478,53 @@
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32">
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35">
         <v>39.0</v>
       </c>
-      <c r="K10" s="41"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="42">
+      <c r="K10" s="44"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="45">
         <v>38.0</v>
       </c>
-      <c r="N10" s="43"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="22"/>
-      <c r="Y10" s="35"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="22"/>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="12"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="5"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="14"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="7"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
-      <c r="AI10" s="6">
+      <c r="AI10" s="8">
         <v>8.0</v>
       </c>
-      <c r="AJ10" s="4" t="s">
-        <v>14</v>
+      <c r="AJ10" s="6" t="s">
+        <v>16</v>
       </c>
-      <c r="AK10" s="17">
+      <c r="AK10" s="19">
         <v>40.0</v>
       </c>
       <c r="AL10" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
@@ -1443,57 +1538,57 @@
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="4"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="46">
+      <c r="H11" s="7"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="49">
         <v>58.0</v>
       </c>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="47">
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="50">
         <v>18.0</v>
       </c>
-      <c r="T11" s="14"/>
-      <c r="U11" s="47">
+      <c r="T11" s="16"/>
+      <c r="U11" s="50">
         <v>18.0</v>
       </c>
-      <c r="V11" s="11"/>
-      <c r="W11" s="47">
+      <c r="V11" s="13"/>
+      <c r="W11" s="50">
         <v>22.0</v>
       </c>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="15"/>
-      <c r="AE11" s="5"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="29"/>
+      <c r="AB11" s="16"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="7"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
-      <c r="AI11" s="6">
+      <c r="AI11" s="8">
         <v>9.0</v>
       </c>
-      <c r="AJ11" s="4" t="s">
-        <v>16</v>
+      <c r="AJ11" s="6" t="s">
+        <v>18</v>
       </c>
-      <c r="AK11" s="17">
+      <c r="AK11" s="19">
         <v>41.0</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
@@ -1512,56 +1607,56 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="48">
+      <c r="H12" s="7"/>
+      <c r="I12" s="51">
         <v>40.0</v>
       </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="52">
+      <c r="J12" s="16"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="55">
         <v>11.0</v>
       </c>
-      <c r="R12" s="53"/>
-      <c r="S12" s="54">
+      <c r="R12" s="56"/>
+      <c r="S12" s="57">
         <v>13.0</v>
       </c>
-      <c r="T12" s="14"/>
-      <c r="U12" s="55">
+      <c r="T12" s="16"/>
+      <c r="U12" s="58">
         <v>18.0</v>
       </c>
-      <c r="V12" s="55">
+      <c r="V12" s="58">
         <v>19.0</v>
       </c>
-      <c r="W12" s="55">
+      <c r="W12" s="58">
         <v>20.0</v>
       </c>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="22"/>
-      <c r="AA12" s="27"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="12"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="5"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="16"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="7"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
-      <c r="AI12" s="6">
+      <c r="AI12" s="8">
         <v>10.0</v>
       </c>
-      <c r="AJ12" s="4" t="s">
-        <v>18</v>
+      <c r="AJ12" s="6" t="s">
+        <v>20</v>
       </c>
-      <c r="AK12" s="17">
+      <c r="AK12" s="19">
         <v>42.0</v>
       </c>
       <c r="AL12" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
@@ -1574,52 +1669,52 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="56" t="s">
-        <v>20</v>
+      <c r="B13" s="59" t="s">
+        <v>22</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="26"/>
-      <c r="Y13" s="26"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="15"/>
-      <c r="AE13" s="5"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="29"/>
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="16"/>
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="16"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="17"/>
+      <c r="AE13" s="7"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
-      <c r="AI13" s="6">
+      <c r="AI13" s="8">
         <v>11.0</v>
       </c>
-      <c r="AJ13" s="4" t="s">
-        <v>21</v>
+      <c r="AJ13" s="6" t="s">
+        <v>23</v>
       </c>
-      <c r="AK13" s="17">
+      <c r="AK13" s="19">
         <v>43.0</v>
       </c>
       <c r="AL13" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
@@ -1633,63 +1728,63 @@
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="57">
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="60">
         <v>8.0</v>
       </c>
-      <c r="N14" s="19"/>
-      <c r="O14" s="13">
+      <c r="N14" s="21"/>
+      <c r="O14" s="15">
         <v>9.0</v>
       </c>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="58">
+      <c r="P14" s="16"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="61">
         <v>15.0</v>
       </c>
-      <c r="U14" s="36">
+      <c r="U14" s="39">
         <v>16.0</v>
       </c>
-      <c r="V14" s="14"/>
-      <c r="W14" s="59"/>
-      <c r="X14" s="60"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="36">
+      <c r="V14" s="16"/>
+      <c r="W14" s="62"/>
+      <c r="X14" s="63"/>
+      <c r="Y14" s="64"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="39">
         <v>21.0</v>
       </c>
-      <c r="AB14" s="14"/>
-      <c r="AC14" s="13">
+      <c r="AB14" s="16"/>
+      <c r="AC14" s="15">
         <v>24.0</v>
       </c>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="5"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="7"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
-      <c r="AI14" s="6">
+      <c r="AI14" s="8">
         <v>12.0</v>
       </c>
-      <c r="AJ14" s="4" t="s">
-        <v>24</v>
+      <c r="AJ14" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="AK14" s="1">
         <v>44.0</v>
       </c>
-      <c r="AL14" s="62" t="s">
-        <v>25</v>
+      <c r="AL14" s="65" t="s">
+        <v>27</v>
       </c>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
@@ -1703,7 +1798,7 @@
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1712,44 +1807,44 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="13">
+      <c r="J15" s="16"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="15">
         <v>10.0</v>
       </c>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="61"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="61"/>
-      <c r="Z15" s="26"/>
-      <c r="AA15" s="26"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="12"/>
-      <c r="AD15" s="15"/>
-      <c r="AE15" s="5"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="64"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="64"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="29"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="7"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
-      <c r="AI15" s="6">
+      <c r="AI15" s="8">
         <v>13.0</v>
       </c>
-      <c r="AJ15" s="4" t="s">
-        <v>27</v>
+      <c r="AJ15" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="AK15" s="1">
         <v>45.0</v>
       </c>
-      <c r="AL15" s="63" t="s">
-        <v>28</v>
+      <c r="AL15" s="66" t="s">
+        <v>30</v>
       </c>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
@@ -1763,7 +1858,7 @@
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1772,44 +1867,44 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="59"/>
-      <c r="V16" s="60"/>
-      <c r="W16" s="67"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="60"/>
-      <c r="Z16" s="60"/>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="14"/>
-      <c r="AC16" s="13">
+      <c r="R16" s="21"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="62"/>
+      <c r="V16" s="63"/>
+      <c r="W16" s="70"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="63"/>
+      <c r="Z16" s="63"/>
+      <c r="AA16" s="64"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="15">
         <v>25.0</v>
       </c>
-      <c r="AD16" s="15"/>
-      <c r="AE16" s="5"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="7"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
-      <c r="AI16" s="6">
+      <c r="AI16" s="8">
         <v>14.0</v>
       </c>
-      <c r="AJ16" s="4" t="s">
-        <v>30</v>
+      <c r="AJ16" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="AK16" s="1">
         <v>46.0</v>
       </c>
       <c r="AL16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
@@ -1823,7 +1918,7 @@
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1832,48 +1927,48 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="46">
+      <c r="J17" s="16"/>
+      <c r="K17" s="49">
         <v>57.0</v>
       </c>
-      <c r="L17" s="43"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="26"/>
-      <c r="Y17" s="26"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="68">
+      <c r="L17" s="46"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="64"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="71">
         <v>27.0</v>
       </c>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="13">
+      <c r="AB17" s="13"/>
+      <c r="AC17" s="72">
         <v>26.0</v>
       </c>
-      <c r="AD17" s="15"/>
-      <c r="AE17" s="5"/>
+      <c r="AD17" s="17"/>
+      <c r="AE17" s="7"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
-      <c r="AI17" s="6">
+      <c r="AI17" s="8">
         <v>15.0</v>
       </c>
-      <c r="AJ17" s="4" t="s">
-        <v>33</v>
+      <c r="AJ17" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="AK17" s="1">
         <v>47.0</v>
       </c>
       <c r="AL17" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
@@ -1887,7 +1982,7 @@
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1896,44 +1991,44 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="66"/>
-      <c r="N18" s="66"/>
-      <c r="O18" s="66"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="13">
+      <c r="J18" s="16"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="74"/>
+      <c r="Q18" s="15">
         <v>12.0</v>
       </c>
-      <c r="R18" s="14"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="60"/>
-      <c r="U18" s="67"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="60"/>
-      <c r="X18" s="60"/>
-      <c r="Y18" s="60"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="60"/>
-      <c r="AB18" s="60"/>
-      <c r="AC18" s="67"/>
-      <c r="AD18" s="15"/>
-      <c r="AE18" s="5"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="63"/>
+      <c r="U18" s="70"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="63"/>
+      <c r="X18" s="63"/>
+      <c r="Y18" s="63"/>
+      <c r="Z18" s="63"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="70"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="7"/>
       <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
-      <c r="AI18" s="6">
+      <c r="AI18" s="8">
         <v>16.0</v>
       </c>
-      <c r="AJ18" s="4" t="s">
-        <v>36</v>
+      <c r="AJ18" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="AK18" s="1">
         <v>48.0</v>
       </c>
       <c r="AL18" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
@@ -1947,7 +2042,7 @@
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1956,46 +2051,46 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="71">
+      <c r="J19" s="16"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="75">
         <v>43.0</v>
       </c>
-      <c r="T19" s="5"/>
-      <c r="U19" s="72" t="s">
-        <v>39</v>
+      <c r="T19" s="7"/>
+      <c r="U19" s="76" t="s">
+        <v>41</v>
       </c>
-      <c r="V19" s="43"/>
-      <c r="W19" s="43"/>
-      <c r="X19" s="43"/>
-      <c r="Y19" s="43"/>
-      <c r="Z19" s="5"/>
-      <c r="AA19" s="5"/>
-      <c r="AB19" s="5"/>
-      <c r="AC19" s="5"/>
-      <c r="AD19" s="5"/>
-      <c r="AE19" s="5"/>
+      <c r="V19" s="46"/>
+      <c r="W19" s="46"/>
+      <c r="X19" s="46"/>
+      <c r="Y19" s="46"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
+      <c r="AE19" s="7"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
-      <c r="AI19" s="6">
+      <c r="AI19" s="8">
         <v>17.0</v>
       </c>
-      <c r="AJ19" s="4" t="s">
-        <v>40</v>
+      <c r="AJ19" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="AK19" s="1">
         <v>49.0</v>
       </c>
       <c r="AL19" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
@@ -2009,7 +2104,7 @@
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -2018,48 +2113,48 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="73">
+      <c r="J20" s="16"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="77">
         <v>42.0</v>
       </c>
-      <c r="N20" s="40"/>
-      <c r="O20" s="6">
+      <c r="N20" s="43"/>
+      <c r="O20" s="8">
         <v>14.0</v>
       </c>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="74"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="75"/>
-      <c r="V20" s="76"/>
-      <c r="W20" s="76"/>
-      <c r="X20" s="77">
+      <c r="P20" s="21"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="78"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="79"/>
+      <c r="V20" s="80"/>
+      <c r="W20" s="80"/>
+      <c r="X20" s="81">
         <v>51.0</v>
       </c>
-      <c r="Y20" s="78"/>
-      <c r="Z20" s="79"/>
-      <c r="AA20" s="80"/>
-      <c r="AB20" s="79"/>
-      <c r="AC20" s="81"/>
-      <c r="AD20" s="15"/>
-      <c r="AE20" s="5"/>
+      <c r="Y20" s="82"/>
+      <c r="Z20" s="83"/>
+      <c r="AA20" s="84"/>
+      <c r="AB20" s="83"/>
+      <c r="AC20" s="85"/>
+      <c r="AD20" s="17"/>
+      <c r="AE20" s="7"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
-      <c r="AI20" s="6">
+      <c r="AI20" s="8">
         <v>18.0</v>
       </c>
-      <c r="AJ20" s="4" t="s">
-        <v>43</v>
+      <c r="AJ20" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="AK20" s="1">
         <v>50.0</v>
       </c>
       <c r="AL20" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
@@ -2073,7 +2168,7 @@
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2082,46 +2177,46 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="38">
+      <c r="J21" s="16"/>
+      <c r="K21" s="41">
         <v>41.0</v>
       </c>
-      <c r="L21" s="43"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="74"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="82"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="43"/>
-      <c r="Y21" s="83"/>
-      <c r="Z21" s="5"/>
-      <c r="AA21" s="82"/>
-      <c r="AB21" s="5"/>
-      <c r="AC21" s="84">
+      <c r="L21" s="46"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="78"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="86"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="46"/>
+      <c r="Y21" s="87"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="86"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="88">
         <v>52.0</v>
       </c>
-      <c r="AD21" s="15"/>
-      <c r="AE21" s="5"/>
+      <c r="AD21" s="17"/>
+      <c r="AE21" s="7"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
-      <c r="AI21" s="6">
+      <c r="AI21" s="8">
         <v>19.0</v>
       </c>
-      <c r="AJ21" s="4" t="s">
-        <v>46</v>
+      <c r="AJ21" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="AK21" s="1">
         <v>51.0</v>
       </c>
       <c r="AL21" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AT21" s="2"/>
     </row>
@@ -2135,52 +2230,52 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="85"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="86"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="87"/>
-      <c r="R22" s="88"/>
-      <c r="S22" s="89">
+      <c r="J22" s="16"/>
+      <c r="K22" s="89"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="90"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="91"/>
+      <c r="R22" s="92"/>
+      <c r="S22" s="93">
         <v>46.0</v>
       </c>
-      <c r="T22" s="5"/>
-      <c r="U22" s="84">
+      <c r="T22" s="7"/>
+      <c r="U22" s="88">
         <v>48.0</v>
       </c>
-      <c r="V22" s="5"/>
-      <c r="W22" s="90">
+      <c r="V22" s="7"/>
+      <c r="W22" s="94">
         <v>50.0</v>
       </c>
-      <c r="X22" s="43"/>
-      <c r="Y22" s="91">
+      <c r="X22" s="46"/>
+      <c r="Y22" s="95">
         <v>53.0</v>
       </c>
-      <c r="Z22" s="43"/>
-      <c r="AA22" s="83"/>
-      <c r="AB22" s="5"/>
-      <c r="AC22" s="92">
+      <c r="Z22" s="46"/>
+      <c r="AA22" s="87"/>
+      <c r="AB22" s="7"/>
+      <c r="AC22" s="96">
         <v>54.0</v>
       </c>
-      <c r="AD22" s="15"/>
-      <c r="AE22" s="5"/>
+      <c r="AD22" s="17"/>
+      <c r="AE22" s="7"/>
       <c r="AF22" s="2"/>
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
-      <c r="AI22" s="6">
+      <c r="AI22" s="8">
         <v>20.0</v>
       </c>
       <c r="AJ22" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AK22" s="1">
         <v>52.0</v>
       </c>
       <c r="AL22" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AT22" s="2"/>
     </row>
@@ -2194,48 +2289,48 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="30">
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="97">
         <v>17.0</v>
       </c>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="43"/>
-      <c r="T23" s="43"/>
-      <c r="U23" s="84"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="84">
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="98"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="46"/>
+      <c r="U23" s="88"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="88">
         <v>49.0</v>
       </c>
-      <c r="X23" s="43"/>
-      <c r="Y23" s="94" t="s">
-        <v>50</v>
+      <c r="X23" s="46"/>
+      <c r="Y23" s="99" t="s">
+        <v>52</v>
       </c>
-      <c r="Z23" s="43"/>
-      <c r="AA23" s="83"/>
-      <c r="AB23" s="5"/>
-      <c r="AC23" s="5"/>
-      <c r="AD23" s="5"/>
-      <c r="AE23" s="5"/>
+      <c r="Z23" s="46"/>
+      <c r="AA23" s="87"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="7"/>
       <c r="AF23" s="2"/>
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
-      <c r="AI23" s="6">
+      <c r="AI23" s="8">
         <v>21.0</v>
       </c>
-      <c r="AJ23" s="4" t="s">
-        <v>51</v>
+      <c r="AJ23" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="AK23" s="1">
         <v>53.0</v>
       </c>
       <c r="AL23" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
@@ -2248,101 +2343,104 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="2"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="6"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="87">
+      <c r="J24" s="100"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="91">
         <v>47.0</v>
       </c>
-      <c r="P24" s="88"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="96"/>
-      <c r="T24" s="76"/>
-      <c r="U24" s="97"/>
-      <c r="V24" s="76"/>
-      <c r="W24" s="98"/>
-      <c r="X24" s="43"/>
-      <c r="Y24" s="43"/>
-      <c r="Z24" s="43"/>
-      <c r="AA24" s="99"/>
-      <c r="AB24" s="100">
+      <c r="P24" s="92"/>
+      <c r="Q24" s="101"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="102"/>
+      <c r="T24" s="80"/>
+      <c r="U24" s="103"/>
+      <c r="V24" s="80"/>
+      <c r="W24" s="104"/>
+      <c r="X24" s="46"/>
+      <c r="Y24" s="95"/>
+      <c r="Z24" s="46"/>
+      <c r="AA24" s="105"/>
+      <c r="AB24" s="106">
         <v>56.0</v>
       </c>
-      <c r="AC24" s="101"/>
-      <c r="AD24" s="15"/>
-      <c r="AE24" s="5"/>
+      <c r="AC24" s="107"/>
+      <c r="AD24" s="17"/>
+      <c r="AE24" s="7"/>
       <c r="AF24" s="2"/>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
-      <c r="AI24" s="6">
+      <c r="AI24" s="8">
         <v>22.0</v>
       </c>
-      <c r="AJ24" s="4" t="s">
-        <v>53</v>
+      <c r="AJ24" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="AK24" s="1">
         <v>54.0</v>
       </c>
       <c r="AL24" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AT24" s="2"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="2"/>
-      <c r="B25" s="4"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="83"/>
-      <c r="T25" s="43"/>
-      <c r="U25" s="43"/>
-      <c r="V25" s="43"/>
-      <c r="W25" s="43"/>
-      <c r="X25" s="43"/>
-      <c r="Z25" s="43"/>
-      <c r="AA25" s="83"/>
-      <c r="AB25" s="5"/>
-      <c r="AC25" s="5"/>
-      <c r="AD25" s="5"/>
-      <c r="AE25" s="5"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="108" t="s">
+        <v>57</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="87"/>
+      <c r="T25" s="46"/>
+      <c r="U25" s="46"/>
+      <c r="V25" s="46"/>
+      <c r="W25" s="46"/>
+      <c r="X25" s="46"/>
+      <c r="Y25" s="87"/>
+      <c r="Z25" s="46"/>
+      <c r="AA25" s="87"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="7"/>
+      <c r="AD25" s="7"/>
+      <c r="AE25" s="7"/>
       <c r="AF25" s="2"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
-      <c r="AI25" s="6">
+      <c r="AI25" s="8">
         <v>23.0</v>
       </c>
-      <c r="AJ25" s="4" t="s">
-        <v>55</v>
+      <c r="AJ25" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="AK25" s="1">
         <v>55.0</v>
       </c>
       <c r="AL25" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
@@ -2351,41 +2449,52 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="102"/>
-      <c r="P26" s="79"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="79"/>
-      <c r="S26" s="98"/>
-      <c r="T26" s="5"/>
-      <c r="Z26" s="43"/>
-      <c r="AA26" s="103"/>
-      <c r="AB26" s="79"/>
-      <c r="AC26" s="104">
+      <c r="H26" s="7"/>
+      <c r="I26" s="109"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="110"/>
+      <c r="P26" s="83"/>
+      <c r="Q26" s="83"/>
+      <c r="R26" s="83"/>
+      <c r="S26" s="104"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="111">
+        <v>61.0</v>
+      </c>
+      <c r="V26" s="81">
+        <v>60.0</v>
+      </c>
+      <c r="W26" s="81">
+        <v>59.0</v>
+      </c>
+      <c r="X26" s="80"/>
+      <c r="Y26" s="104"/>
+      <c r="Z26" s="46"/>
+      <c r="AA26" s="112"/>
+      <c r="AB26" s="83"/>
+      <c r="AC26" s="113">
         <v>55.0</v>
       </c>
-      <c r="AD26" s="15"/>
-      <c r="AE26" s="5"/>
+      <c r="AD26" s="17"/>
+      <c r="AE26" s="7"/>
       <c r="AF26" s="2"/>
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
-      <c r="AI26" s="6">
+      <c r="AI26" s="8">
         <v>24.0</v>
       </c>
-      <c r="AJ26" s="4" t="s">
-        <v>57</v>
+      <c r="AJ26" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="AK26" s="1">
         <v>56.0</v>
       </c>
-      <c r="AL26" s="105" t="s">
-        <v>58</v>
+      <c r="AL26" s="114" t="s">
+        <v>61</v>
       </c>
       <c r="AT26" s="2"/>
     </row>
@@ -2397,48 +2506,48 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="106" t="s">
-        <v>59</v>
+      <c r="H27" s="7"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="115" t="s">
+        <v>62</v>
       </c>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="107"/>
-      <c r="T27" s="5"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="116"/>
+      <c r="T27" s="7"/>
       <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="2"/>
-      <c r="Z27" s="5"/>
-      <c r="AA27" s="106" t="s">
-        <v>60</v>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="17"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="115" t="s">
+        <v>63</v>
       </c>
-      <c r="AB27" s="15"/>
-      <c r="AC27" s="15"/>
-      <c r="AD27" s="5"/>
-      <c r="AE27" s="5"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="17"/>
+      <c r="AD27" s="7"/>
+      <c r="AE27" s="7"/>
       <c r="AF27" s="2"/>
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
-      <c r="AI27" s="6">
+      <c r="AI27" s="8">
         <v>25.0</v>
       </c>
-      <c r="AJ27" s="4" t="s">
-        <v>61</v>
+      <c r="AJ27" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="AK27" s="1">
         <v>57.0</v>
       </c>
       <c r="AL27" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
@@ -2457,41 +2566,43 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="43"/>
-      <c r="T28" s="43"/>
-      <c r="V28" s="2"/>
-      <c r="Y28" s="2"/>
-      <c r="Z28" s="5"/>
-      <c r="AA28" s="5"/>
-      <c r="AB28" s="5"/>
-      <c r="AC28" s="43"/>
-      <c r="AD28" s="5"/>
-      <c r="AE28" s="2"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="46"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="46"/>
+      <c r="X28" s="46"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="7"/>
+      <c r="AB28" s="7"/>
+      <c r="AC28" s="46"/>
+      <c r="AD28" s="7"/>
+      <c r="AE28" s="117"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
-      <c r="AI28" s="6">
+      <c r="AI28" s="8">
         <v>26.0</v>
       </c>
-      <c r="AJ28" s="8" t="s">
-        <v>63</v>
+      <c r="AJ28" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="AK28" s="1">
         <v>58.0</v>
       </c>
       <c r="AL28" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AM28" s="2"/>
       <c r="AN28" s="2"/>
@@ -2521,9 +2632,9 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="V29" s="2"/>
-      <c r="W29" s="15"/>
-      <c r="X29" s="4" t="s">
-        <v>65</v>
+      <c r="W29" s="17"/>
+      <c r="X29" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
@@ -2534,14 +2645,18 @@
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
       <c r="AH29" s="2"/>
-      <c r="AI29" s="6">
+      <c r="AI29" s="8">
         <v>27.0</v>
       </c>
-      <c r="AJ29" s="4" t="s">
-        <v>66</v>
+      <c r="AJ29" s="6" t="s">
+        <v>69</v>
       </c>
-      <c r="AK29" s="2"/>
-      <c r="AL29" s="2"/>
+      <c r="AK29" s="1">
+        <v>59.0</v>
+      </c>
+      <c r="AL29" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="AM29" s="2"/>
       <c r="AN29" s="2"/>
       <c r="AO29" s="2"/>
@@ -2554,18 +2669,18 @@
     <row r="30" ht="13.5" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
-      <c r="D30" s="108" t="s">
-        <v>50</v>
+      <c r="D30" s="118" t="s">
+        <v>52</v>
       </c>
-      <c r="E30" s="108" t="s">
-        <v>67</v>
+      <c r="E30" s="118" t="s">
+        <v>71</v>
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="V30" s="2"/>
-      <c r="W30" s="59"/>
-      <c r="X30" s="4" t="s">
-        <v>68</v>
+      <c r="W30" s="62"/>
+      <c r="X30" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
@@ -2577,11 +2692,17 @@
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
       <c r="AH30" s="2"/>
-      <c r="AI30" s="6">
+      <c r="AI30" s="8">
         <v>28.0</v>
       </c>
-      <c r="AJ30" s="4" t="s">
-        <v>69</v>
+      <c r="AJ30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK30" s="118">
+        <v>60.0</v>
+      </c>
+      <c r="AL30" s="118" t="s">
+        <v>74</v>
       </c>
       <c r="AM30" s="2"/>
       <c r="AN30" s="2"/>
@@ -2595,12 +2716,18 @@
     <row r="31" ht="13.5" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
+      <c r="D31" s="118" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="118" t="s">
+        <v>75</v>
+      </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="V31" s="2"/>
-      <c r="W31" s="109"/>
-      <c r="X31" s="4" t="s">
-        <v>70</v>
+      <c r="W31" s="119"/>
+      <c r="X31" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
@@ -2611,11 +2738,17 @@
       <c r="AF31" s="2"/>
       <c r="AG31" s="2"/>
       <c r="AH31" s="2"/>
-      <c r="AI31" s="6">
+      <c r="AI31" s="8">
         <v>29.0</v>
       </c>
-      <c r="AJ31" s="4" t="s">
-        <v>71</v>
+      <c r="AJ31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK31" s="118">
+        <v>61.0</v>
+      </c>
+      <c r="AL31" s="118" t="s">
+        <v>78</v>
       </c>
       <c r="AM31" s="2"/>
       <c r="AN31" s="2"/>
@@ -2646,9 +2779,9 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="V32" s="2"/>
-      <c r="W32" s="24"/>
-      <c r="X32" s="4" t="s">
-        <v>72</v>
+      <c r="W32" s="27"/>
+      <c r="X32" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
@@ -2659,11 +2792,11 @@
       <c r="AF32" s="2"/>
       <c r="AG32" s="2"/>
       <c r="AH32" s="2"/>
-      <c r="AI32" s="6">
+      <c r="AI32" s="8">
         <v>30.0</v>
       </c>
-      <c r="AJ32" s="4" t="s">
-        <v>73</v>
+      <c r="AJ32" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="AK32" s="2"/>
       <c r="AL32" s="2"/>
@@ -2698,9 +2831,9 @@
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
-      <c r="W33" s="110"/>
+      <c r="W33" s="120"/>
       <c r="X33" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
@@ -2712,11 +2845,11 @@
       <c r="AF33" s="2"/>
       <c r="AG33" s="2"/>
       <c r="AH33" s="2"/>
-      <c r="AI33" s="6">
+      <c r="AI33" s="8">
         <v>31.0</v>
       </c>
-      <c r="AJ33" s="4" t="s">
-        <v>75</v>
+      <c r="AJ33" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="AK33" s="2"/>
       <c r="AL33" s="2"/>
@@ -2751,9 +2884,9 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
-      <c r="W34" s="111"/>
+      <c r="W34" s="121"/>
       <c r="X34" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
@@ -2765,11 +2898,11 @@
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
-      <c r="AI34" s="6">
+      <c r="AI34" s="8">
         <v>32.0</v>
       </c>
-      <c r="AJ34" s="4" t="s">
-        <v>77</v>
+      <c r="AJ34" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="AK34" s="2"/>
       <c r="AL34" s="2"/>
@@ -2783,8 +2916,8 @@
       <c r="AT34" s="2"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="S35" s="112" t="s">
-        <v>78</v>
+      <c r="S35" s="122" t="s">
+        <v>85</v>
       </c>
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
@@ -2801,7 +2934,7 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
@@ -2817,11 +2950,11 @@
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
-      <c r="AI37" s="17"/>
+      <c r="AI37" s="19"/>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="2"/>
       <c r="AL37" s="2"/>
@@ -2836,11 +2969,11 @@
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
-      <c r="AI38" s="17"/>
+      <c r="AI38" s="19"/>
       <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
       <c r="AL38" s="2"/>
@@ -2855,11 +2988,11 @@
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
-      <c r="AI39" s="17"/>
+      <c r="AI39" s="19"/>
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
       <c r="AL39" s="1"/>
@@ -2874,11 +3007,11 @@
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="AG40" s="2"/>
       <c r="AH40" s="2"/>
-      <c r="AI40" s="17"/>
+      <c r="AI40" s="19"/>
       <c r="AJ40" s="2"/>
       <c r="AK40" s="2"/>
       <c r="AL40" s="2"/>
@@ -2893,11 +3026,11 @@
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
-      <c r="AI41" s="17"/>
+      <c r="AI41" s="19"/>
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
       <c r="AL41" s="2"/>
@@ -2912,11 +3045,11 @@
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
-      <c r="AI42" s="17"/>
+      <c r="AI42" s="19"/>
       <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
       <c r="AL42" s="2"/>
@@ -2930,6 +3063,9 @@
       <c r="AT42" s="2"/>
     </row>
     <row r="43" ht="13.5" customHeight="1">
+      <c r="A43" s="118" t="s">
+        <v>93</v>
+      </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2962,7 +3098,7 @@
       <c r="AF43" s="2"/>
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
-      <c r="AI43" s="17"/>
+      <c r="AI43" s="19"/>
       <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
       <c r="AL43" s="2"/>
@@ -2976,14 +3112,9 @@
       <c r="AT43" s="2"/>
     </row>
     <row r="44" ht="13.5" customHeight="1">
-      <c r="B44" s="113"/>
-      <c r="C44" s="114" t="s">
-        <v>86</v>
+      <c r="A44" s="118" t="s">
+        <v>94</v>
       </c>
-      <c r="D44" s="113"/>
-      <c r="E44" s="113"/>
-      <c r="F44" s="113"/>
-      <c r="G44" s="113"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -3011,7 +3142,7 @@
       <c r="AF44" s="2"/>
       <c r="AG44" s="2"/>
       <c r="AH44" s="2"/>
-      <c r="AI44" s="17"/>
+      <c r="AI44" s="19"/>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="2"/>
       <c r="AL44" s="2"/>
@@ -3025,14 +3156,6 @@
       <c r="AT44" s="2"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="B45" s="113"/>
-      <c r="C45" s="114" t="s">
-        <v>87</v>
-      </c>
-      <c r="D45" s="113"/>
-      <c r="E45" s="113"/>
-      <c r="F45" s="113"/>
-      <c r="G45" s="113"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -3060,7 +3183,7 @@
       <c r="AF45" s="2"/>
       <c r="AG45" s="2"/>
       <c r="AH45" s="2"/>
-      <c r="AI45" s="17"/>
+      <c r="AI45" s="19"/>
       <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
       <c r="AL45" s="2"/>
@@ -3108,7 +3231,7 @@
       <c r="AG46" s="2"/>
       <c r="AH46" s="2"/>
       <c r="AI46" s="1"/>
-      <c r="AJ46" s="62"/>
+      <c r="AJ46" s="65"/>
       <c r="AK46" s="2"/>
       <c r="AL46" s="2"/>
       <c r="AM46" s="2"/>
@@ -3121,12 +3244,6 @@
       <c r="AT46" s="2"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -3168,12 +3285,6 @@
       <c r="AT47" s="2"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -3643,7 +3754,7 @@
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
       <c r="AI58" s="1"/>
-      <c r="AJ58" s="105"/>
+      <c r="AJ58" s="114"/>
       <c r="AR58" s="2"/>
       <c r="AS58" s="2"/>
       <c r="AT58" s="2"/>

</xml_diff>

<commit_message>
Small edits to _30, _40, and _42 files. Updated map
</commit_message>
<xml_diff>
--- a/Krieger Kastle.xlsx
+++ b/Krieger Kastle.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
   <si>
     <t>
 </t>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>pinata</t>
+  </si>
+  <si>
+    <t>Key ^</t>
   </si>
   <si>
     <t>Door East, need key</t>
@@ -116,7 +119,10 @@
     <t>Poisocaine Pen</t>
   </si>
   <si>
-    <t>Rabbert</t>
+    <t>Rabbert Klein</t>
+  </si>
+  <si>
+    <t>Card \/</t>
   </si>
   <si>
     <t>Weekly Spyglass</t>
@@ -137,7 +143,7 @@
     <t>Krieger (human)</t>
   </si>
   <si>
-    <t>43 Requires Bomb to go south</t>
+    <t>&lt; Bomb</t>
   </si>
   <si>
     <t>Missing 2112 album, moving bookshelf</t>
@@ -170,6 +176,9 @@
     <t>Compusave Multimedia Center</t>
   </si>
   <si>
+    <t>&lt; Record</t>
+  </si>
+  <si>
     <t>R</t>
   </si>
   <si>
@@ -186,6 +195,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>\/ Prism</t>
   </si>
   <si>
     <t>cesta</t>
@@ -209,13 +221,16 @@
     <t>wooden device with wheel</t>
   </si>
   <si>
-    <t>tanning bed (using it kills you)</t>
+    <t>tanning bed (Heals kidney wound, else it kills)</t>
   </si>
   <si>
     <t>door, stick</t>
   </si>
   <si>
     <t>game room (skeeball, token machine)</t>
+  </si>
+  <si>
+    <t>Big Robot, Release and wait for octopus</t>
   </si>
   <si>
     <t>Death if you walk here</t>
@@ -227,7 +242,7 @@
     <t>Rush concept album</t>
   </si>
   <si>
-    <t>Big Robot</t>
+    <t>Mitsuko, "use spoon"</t>
   </si>
   <si>
     <t>Cave</t>
@@ -237,9 +252,6 @@
   </si>
   <si>
     <t>clicker (can't pick up)</t>
-  </si>
-  <si>
-    <t>Mitsuko, gives you spoon and wants kidneys in return</t>
   </si>
   <si>
     <t>Van</t>
@@ -257,10 +269,22 @@
     <t>computer monitor in room, dim green</t>
   </si>
   <si>
+    <t>mirror</t>
+  </si>
+  <si>
+    <t>The end takes you to the bash prompt, just like 'quit'</t>
+  </si>
+  <si>
     <t>Lab</t>
   </si>
   <si>
     <t>mare's leg, dry ice, cooler (can't pick up)</t>
+  </si>
+  <si>
+    <t>Ticket Desk</t>
+  </si>
+  <si>
+    <t>Use the prism on pedestal to open end</t>
   </si>
   <si>
     <t>City</t>
@@ -269,10 +293,19 @@
     <t>Deadly Velvet poster</t>
   </si>
   <si>
-    <t>Everything else is mostly Krieger's Kastle or cliffs</t>
+    <t>Boulder</t>
+  </si>
+  <si>
+    <t>Hell</t>
+  </si>
+  <si>
+    <t>Peer review, pit, ladder, hill</t>
   </si>
   <si>
     <t>you can construct a dry ice bomb with a bottle, water, dry ice, and bottlecap (fill bottle with water from pond at 16, 'use ice on beer', 'use cap on bomb', RUN)</t>
+  </si>
+  <si>
+    <t>Prism, Take to 61</t>
   </si>
   <si>
     <t>having three people hold down the console buttons at 38/40/42 releases a murderous octopus from the cryo chamber ('push button'), it heads for the giant robot at R</t>
@@ -297,6 +330,15 @@
   </si>
   <si>
     <t>Missing rush album is at 59. Bring it back past the giant robot, collapsing cave, and cave door (good luck) and place it at 17 to reveal a new path</t>
+  </si>
+  <si>
+    <t>To get past Mitsuko, 'use spoon' while in the room. You will die two minutes after doing this</t>
+  </si>
+  <si>
+    <t>In peer review room, you can 'climb ladder' to go west, or 'climb hill' to escape back south.</t>
+  </si>
+  <si>
+    <t>when shopkeeper at 52 is killed with a bomb you can steal a game but die and A demon calls out in the distance, "r9nV5NXQ2tXXseDX0OSUkIyv4drTudri0ZWF0NTW08jVktTP2IHg247G1ebe18fW5tGOjM3hz5WHjZs=".  The ground opens up below you! You are falling down a bottomless pit......Splat. It wasn't so bottomless after all.</t>
   </si>
 </sst>
 </file>
@@ -330,7 +372,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,12 +401,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC27BA0"/>
-        <bgColor rgb="FFC27BA0"/>
       </patternFill>
     </fill>
     <fill>
@@ -399,12 +435,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEA9999"/>
+        <bgColor rgb="FFEA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE69138"/>
         <bgColor rgb="FFE69138"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC27BA0"/>
+        <bgColor rgb="FFC27BA0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -509,6 +563,32 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="dashed">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dashed">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -591,11 +671,23 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dashed">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="134">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -632,7 +724,7 @@
     <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -656,7 +748,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -665,28 +757,31 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -698,82 +793,88 @@
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="5" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="5" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="6" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="7" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="8" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="8" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="9" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="12" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -788,71 +889,77 @@
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="8" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="6" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="2" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="13" fillId="11" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="10" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="16" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="8" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="5" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="6" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="13" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="13" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="10" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="13" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="10" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="7" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="8" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="8" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="13" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="5" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -864,50 +971,62 @@
     <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="16" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="8" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="13" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="9" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="8" fillId="12" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="13" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="13" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="6" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="12" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="3" fillId="12" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="13" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="13" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="13" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="13" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="19" fillId="13" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="3" fillId="12" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="17" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="13" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="18" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="11" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="13" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="19" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -917,24 +1036,28 @@
       <alignment/>
     </xf>
     <xf borderId="10" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
     <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1298,25 +1421,29 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="28"/>
+      <c r="I7" s="28">
+        <v>2.0</v>
+      </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="M7" s="29" t="s">
+        <v>11</v>
+      </c>
       <c r="N7" s="16"/>
       <c r="O7" s="14"/>
       <c r="P7" s="7"/>
-      <c r="Q7" s="29"/>
+      <c r="Q7" s="30"/>
       <c r="R7" s="13"/>
-      <c r="S7" s="30"/>
+      <c r="S7" s="31"/>
       <c r="T7" s="13"/>
-      <c r="U7" s="30"/>
+      <c r="U7" s="31"/>
       <c r="V7" s="16"/>
-      <c r="W7" s="30"/>
+      <c r="W7" s="31"/>
       <c r="X7" s="7"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
       <c r="AB7" s="16"/>
       <c r="AC7" s="15">
         <v>33.0</v>
@@ -1330,7 +1457,7 @@
         <v>5.0</v>
       </c>
       <c r="AJ7" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AK7" s="19">
         <v>37.0</v>
@@ -1352,19 +1479,17 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32">
+      <c r="G8" s="32"/>
+      <c r="H8" s="33">
         <v>1.0</v>
       </c>
-      <c r="I8" s="33">
-        <v>2.0</v>
-      </c>
+      <c r="I8" s="34"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="35">
+      <c r="K8" s="35"/>
+      <c r="L8" s="36">
         <v>36.0</v>
       </c>
-      <c r="M8" s="36">
+      <c r="M8" s="37">
         <v>45.0</v>
       </c>
       <c r="N8" s="16"/>
@@ -1372,25 +1497,25 @@
         <v>7.0</v>
       </c>
       <c r="P8" s="16"/>
-      <c r="Q8" s="37">
+      <c r="Q8" s="38">
         <v>28.0</v>
       </c>
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
       <c r="T8" s="25"/>
-      <c r="U8" s="38"/>
+      <c r="U8" s="39"/>
       <c r="V8" s="16"/>
-      <c r="W8" s="39">
+      <c r="W8" s="40">
         <v>30.0</v>
       </c>
       <c r="X8" s="16"/>
-      <c r="Y8" s="37">
+      <c r="Y8" s="38">
         <v>23.0</v>
       </c>
       <c r="Z8" s="25"/>
-      <c r="AA8" s="30"/>
+      <c r="AA8" s="31"/>
       <c r="AB8" s="16"/>
-      <c r="AC8" s="40"/>
+      <c r="AC8" s="41"/>
       <c r="AD8" s="17"/>
       <c r="AE8" s="7"/>
       <c r="AF8" s="2"/>
@@ -1400,13 +1525,13 @@
         <v>6.0</v>
       </c>
       <c r="AJ8" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AK8" s="19">
         <v>38.0</v>
       </c>
       <c r="AL8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
@@ -1428,27 +1553,27 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="16"/>
-      <c r="K9" s="41">
+      <c r="K9" s="42">
         <v>44.0</v>
       </c>
       <c r="L9" s="16"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="44"/>
       <c r="O9" s="14"/>
       <c r="P9" s="16"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
       <c r="V9" s="7"/>
-      <c r="W9" s="29"/>
+      <c r="W9" s="30"/>
       <c r="X9" s="13"/>
-      <c r="Y9" s="30"/>
+      <c r="Y9" s="31"/>
       <c r="Z9" s="16"/>
-      <c r="AA9" s="30"/>
-      <c r="AB9" s="29"/>
-      <c r="AC9" s="29"/>
+      <c r="AA9" s="31"/>
+      <c r="AB9" s="30"/>
+      <c r="AC9" s="30"/>
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
       <c r="AF9" s="2"/>
@@ -1458,13 +1583,13 @@
         <v>7.0</v>
       </c>
       <c r="AJ9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AK9" s="19">
         <v>39.0</v>
       </c>
       <c r="AL9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
@@ -1484,27 +1609,27 @@
       <c r="F10" s="2"/>
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="35">
+      <c r="I10" s="35"/>
+      <c r="J10" s="36">
         <v>39.0</v>
       </c>
-      <c r="K10" s="44"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="16"/>
-      <c r="M10" s="45">
+      <c r="M10" s="46">
         <v>38.0</v>
       </c>
-      <c r="N10" s="46"/>
-      <c r="O10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="48"/>
       <c r="P10" s="16"/>
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
       <c r="S10" s="27"/>
       <c r="T10" s="25"/>
-      <c r="U10" s="30"/>
+      <c r="U10" s="31"/>
       <c r="V10" s="16"/>
       <c r="W10" s="27"/>
       <c r="X10" s="25"/>
-      <c r="Y10" s="38"/>
+      <c r="Y10" s="39"/>
       <c r="Z10" s="16"/>
       <c r="AA10" s="25"/>
       <c r="AB10" s="25"/>
@@ -1518,13 +1643,13 @@
         <v>8.0</v>
       </c>
       <c r="AJ10" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AK10" s="19">
         <v>40.0</v>
       </c>
       <c r="AL10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
@@ -1544,33 +1669,33 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="48"/>
+      <c r="I11" s="49"/>
       <c r="J11" s="16"/>
-      <c r="K11" s="49">
+      <c r="K11" s="50">
         <v>58.0</v>
       </c>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="48"/>
       <c r="P11" s="7"/>
-      <c r="Q11" s="29"/>
+      <c r="Q11" s="30"/>
       <c r="R11" s="13"/>
-      <c r="S11" s="50">
+      <c r="S11" s="51">
         <v>18.0</v>
       </c>
       <c r="T11" s="16"/>
-      <c r="U11" s="50">
+      <c r="U11" s="51">
         <v>18.0</v>
       </c>
       <c r="V11" s="13"/>
-      <c r="W11" s="50">
+      <c r="W11" s="51">
         <v>22.0</v>
       </c>
-      <c r="X11" s="29"/>
-      <c r="Y11" s="29"/>
-      <c r="Z11" s="29"/>
-      <c r="AA11" s="29"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="30"/>
+      <c r="AA11" s="30"/>
       <c r="AB11" s="16"/>
       <c r="AC11" s="14"/>
       <c r="AD11" s="17"/>
@@ -1582,13 +1707,13 @@
         <v>9.0</v>
       </c>
       <c r="AJ11" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AK11" s="19">
         <v>41.0</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
@@ -1608,37 +1733,37 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="51">
+      <c r="I12" s="52">
         <v>40.0</v>
       </c>
       <c r="J12" s="16"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="40"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="41"/>
       <c r="P12" s="16"/>
-      <c r="Q12" s="55">
+      <c r="Q12" s="56">
         <v>11.0</v>
       </c>
-      <c r="R12" s="56"/>
-      <c r="S12" s="57">
+      <c r="R12" s="57"/>
+      <c r="S12" s="58">
         <v>13.0</v>
       </c>
       <c r="T12" s="16"/>
-      <c r="U12" s="58">
+      <c r="U12" s="59">
         <v>18.0</v>
       </c>
-      <c r="V12" s="58">
+      <c r="V12" s="59">
         <v>19.0</v>
       </c>
-      <c r="W12" s="58">
+      <c r="W12" s="59">
         <v>20.0</v>
       </c>
       <c r="X12" s="25"/>
       <c r="Y12" s="25"/>
       <c r="Z12" s="25"/>
-      <c r="AA12" s="30"/>
+      <c r="AA12" s="31"/>
       <c r="AB12" s="16"/>
       <c r="AC12" s="14"/>
       <c r="AD12" s="17"/>
@@ -1650,13 +1775,13 @@
         <v>10.0</v>
       </c>
       <c r="AJ12" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AK12" s="19">
         <v>42.0</v>
       </c>
       <c r="AL12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
@@ -1669,34 +1794,34 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="59" t="s">
-        <v>22</v>
+      <c r="B13" s="60" t="s">
+        <v>23</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
       <c r="P13" s="16"/>
-      <c r="Q13" s="30"/>
+      <c r="Q13" s="31"/>
       <c r="R13" s="7"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
       <c r="V13" s="7"/>
-      <c r="W13" s="29"/>
-      <c r="X13" s="29"/>
-      <c r="Y13" s="29"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
       <c r="Z13" s="16"/>
-      <c r="AA13" s="30"/>
+      <c r="AA13" s="31"/>
       <c r="AB13" s="16"/>
       <c r="AC13" s="14"/>
       <c r="AD13" s="17"/>
@@ -1708,13 +1833,13 @@
         <v>11.0</v>
       </c>
       <c r="AJ13" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AK13" s="19">
         <v>43.0</v>
       </c>
       <c r="AL13" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
@@ -1728,19 +1853,23 @@
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="61">
+        <v>66.0</v>
+      </c>
+      <c r="I14" s="62">
+        <v>65.0</v>
+      </c>
       <c r="J14" s="16"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="60">
+      <c r="K14" s="43"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="63">
         <v>8.0</v>
       </c>
       <c r="N14" s="21"/>
@@ -1751,18 +1880,18 @@
       <c r="Q14" s="14"/>
       <c r="R14" s="16"/>
       <c r="S14" s="27"/>
-      <c r="T14" s="61">
+      <c r="T14" s="64">
         <v>15.0</v>
       </c>
-      <c r="U14" s="39">
+      <c r="U14" s="40">
         <v>16.0</v>
       </c>
       <c r="V14" s="16"/>
-      <c r="W14" s="62"/>
-      <c r="X14" s="63"/>
-      <c r="Y14" s="64"/>
+      <c r="W14" s="65"/>
+      <c r="X14" s="66"/>
+      <c r="Y14" s="67"/>
       <c r="Z14" s="16"/>
-      <c r="AA14" s="39">
+      <c r="AA14" s="40">
         <v>21.0</v>
       </c>
       <c r="AB14" s="16"/>
@@ -1778,13 +1907,13 @@
         <v>12.0</v>
       </c>
       <c r="AJ14" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AK14" s="1">
         <v>44.0</v>
       </c>
-      <c r="AL14" s="65" t="s">
-        <v>27</v>
+      <c r="AL14" s="68" t="s">
+        <v>28</v>
       </c>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
@@ -1798,19 +1927,19 @@
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="69"/>
       <c r="J15" s="16"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="29"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="30"/>
       <c r="N15" s="16"/>
       <c r="O15" s="15">
         <v>10.0</v>
@@ -1820,13 +1949,13 @@
       <c r="R15" s="13"/>
       <c r="S15" s="14"/>
       <c r="T15" s="7"/>
-      <c r="U15" s="29"/>
+      <c r="U15" s="30"/>
       <c r="V15" s="13"/>
-      <c r="W15" s="64"/>
+      <c r="W15" s="67"/>
       <c r="X15" s="16"/>
-      <c r="Y15" s="64"/>
-      <c r="Z15" s="29"/>
-      <c r="AA15" s="29"/>
+      <c r="Y15" s="67"/>
+      <c r="Z15" s="30"/>
+      <c r="AA15" s="30"/>
       <c r="AB15" s="16"/>
       <c r="AC15" s="14"/>
       <c r="AD15" s="17"/>
@@ -1838,13 +1967,13 @@
         <v>13.0</v>
       </c>
       <c r="AJ15" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AK15" s="1">
         <v>45.0</v>
       </c>
-      <c r="AL15" s="66" t="s">
-        <v>30</v>
+      <c r="AL15" s="70" t="s">
+        <v>31</v>
       </c>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
@@ -1858,33 +1987,33 @@
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="69"/>
       <c r="J16" s="16"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="43"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="72"/>
+      <c r="M16" s="73"/>
+      <c r="N16" s="44"/>
       <c r="O16" s="21"/>
       <c r="P16" s="21"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="21"/>
-      <c r="S16" s="40"/>
+      <c r="S16" s="41"/>
       <c r="T16" s="16"/>
-      <c r="U16" s="62"/>
-      <c r="V16" s="63"/>
-      <c r="W16" s="70"/>
+      <c r="U16" s="65"/>
+      <c r="V16" s="66"/>
+      <c r="W16" s="74"/>
       <c r="X16" s="16"/>
-      <c r="Y16" s="63"/>
-      <c r="Z16" s="63"/>
-      <c r="AA16" s="64"/>
+      <c r="Y16" s="66"/>
+      <c r="Z16" s="66"/>
+      <c r="AA16" s="67"/>
       <c r="AB16" s="16"/>
       <c r="AC16" s="15">
         <v>25.0</v>
@@ -1898,13 +2027,13 @@
         <v>14.0</v>
       </c>
       <c r="AJ16" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AK16" s="1">
         <v>46.0</v>
       </c>
       <c r="AL16" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
@@ -1917,40 +2046,42 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
-        <v>34</v>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="69"/>
       <c r="J17" s="16"/>
-      <c r="K17" s="49">
+      <c r="K17" s="50">
         <v>57.0</v>
       </c>
-      <c r="L17" s="46"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="75" t="s">
+        <v>36</v>
+      </c>
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="7"/>
-      <c r="S17" s="29"/>
+      <c r="S17" s="30"/>
       <c r="T17" s="13"/>
-      <c r="U17" s="64"/>
+      <c r="U17" s="67"/>
       <c r="V17" s="7"/>
-      <c r="W17" s="29"/>
-      <c r="X17" s="29"/>
-      <c r="Y17" s="29"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="30"/>
       <c r="Z17" s="13"/>
-      <c r="AA17" s="71">
+      <c r="AA17" s="76">
         <v>27.0</v>
       </c>
       <c r="AB17" s="13"/>
-      <c r="AC17" s="72">
+      <c r="AC17" s="77">
         <v>26.0</v>
       </c>
       <c r="AD17" s="17"/>
@@ -1962,13 +2093,13 @@
         <v>15.0</v>
       </c>
       <c r="AJ17" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AK17" s="1">
         <v>47.0</v>
       </c>
       <c r="AL17" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
@@ -1982,37 +2113,37 @@
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="69"/>
       <c r="J18" s="16"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="74"/>
+      <c r="K18" s="78"/>
+      <c r="L18" s="72"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="79"/>
       <c r="Q18" s="15">
         <v>12.0</v>
       </c>
       <c r="R18" s="16"/>
-      <c r="S18" s="62"/>
-      <c r="T18" s="63"/>
-      <c r="U18" s="70"/>
+      <c r="S18" s="65"/>
+      <c r="T18" s="66"/>
+      <c r="U18" s="74"/>
       <c r="V18" s="16"/>
-      <c r="W18" s="63"/>
-      <c r="X18" s="63"/>
-      <c r="Y18" s="63"/>
-      <c r="Z18" s="63"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="70"/>
+      <c r="W18" s="66"/>
+      <c r="X18" s="66"/>
+      <c r="Y18" s="66"/>
+      <c r="Z18" s="66"/>
+      <c r="AA18" s="66"/>
+      <c r="AB18" s="66"/>
+      <c r="AC18" s="74"/>
       <c r="AD18" s="17"/>
       <c r="AE18" s="7"/>
       <c r="AF18" s="2"/>
@@ -2022,13 +2153,13 @@
         <v>16.0</v>
       </c>
       <c r="AJ18" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AK18" s="1">
         <v>48.0</v>
       </c>
       <c r="AL18" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
@@ -2042,35 +2173,37 @@
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="80">
+        <v>64.0</v>
+      </c>
       <c r="J19" s="16"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="29"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="30"/>
       <c r="N19" s="7"/>
-      <c r="O19" s="29"/>
+      <c r="O19" s="30"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="14"/>
       <c r="R19" s="7"/>
-      <c r="S19" s="75">
+      <c r="S19" s="81">
         <v>43.0</v>
       </c>
-      <c r="T19" s="7"/>
-      <c r="U19" s="76" t="s">
-        <v>41</v>
+      <c r="T19" s="29" t="s">
+        <v>43</v>
       </c>
-      <c r="V19" s="46"/>
-      <c r="W19" s="46"/>
-      <c r="X19" s="46"/>
-      <c r="Y19" s="46"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="47"/>
+      <c r="W19" s="47"/>
+      <c r="X19" s="47"/>
+      <c r="Y19" s="47"/>
       <c r="Z19" s="7"/>
       <c r="AA19" s="7"/>
       <c r="AB19" s="7"/>
@@ -2084,13 +2217,13 @@
         <v>17.0</v>
       </c>
       <c r="AJ19" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AK19" s="1">
         <v>49.0</v>
       </c>
       <c r="AL19" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
@@ -2104,41 +2237,41 @@
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="69"/>
       <c r="J20" s="16"/>
-      <c r="K20" s="67"/>
-      <c r="L20" s="68"/>
-      <c r="M20" s="77">
+      <c r="K20" s="71"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="82">
         <v>42.0</v>
       </c>
-      <c r="N20" s="43"/>
+      <c r="N20" s="44"/>
       <c r="O20" s="8">
         <v>14.0</v>
       </c>
       <c r="P20" s="21"/>
-      <c r="Q20" s="40"/>
+      <c r="Q20" s="41"/>
       <c r="R20" s="7"/>
-      <c r="S20" s="78"/>
+      <c r="S20" s="83"/>
       <c r="T20" s="7"/>
-      <c r="U20" s="79"/>
-      <c r="V20" s="80"/>
-      <c r="W20" s="80"/>
-      <c r="X20" s="81">
+      <c r="U20" s="84"/>
+      <c r="V20" s="85"/>
+      <c r="W20" s="85"/>
+      <c r="X20" s="86">
         <v>51.0</v>
       </c>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="83"/>
-      <c r="AA20" s="84"/>
-      <c r="AB20" s="83"/>
-      <c r="AC20" s="85"/>
+      <c r="Y20" s="87"/>
+      <c r="Z20" s="88"/>
+      <c r="AA20" s="89"/>
+      <c r="AB20" s="88"/>
+      <c r="AC20" s="90"/>
       <c r="AD20" s="17"/>
       <c r="AE20" s="7"/>
       <c r="AF20" s="2"/>
@@ -2148,13 +2281,13 @@
         <v>18.0</v>
       </c>
       <c r="AJ20" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AK20" s="1">
         <v>50.0</v>
       </c>
       <c r="AL20" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
@@ -2168,37 +2301,37 @@
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="69"/>
       <c r="J21" s="16"/>
-      <c r="K21" s="41">
+      <c r="K21" s="42">
         <v>41.0</v>
       </c>
-      <c r="L21" s="46"/>
-      <c r="M21" s="29"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="30"/>
       <c r="N21" s="13"/>
       <c r="O21" s="14"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
-      <c r="S21" s="78"/>
+      <c r="S21" s="83"/>
       <c r="T21" s="7"/>
-      <c r="U21" s="86"/>
+      <c r="U21" s="91"/>
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
-      <c r="X21" s="46"/>
-      <c r="Y21" s="87"/>
+      <c r="X21" s="47"/>
+      <c r="Y21" s="92"/>
       <c r="Z21" s="7"/>
-      <c r="AA21" s="86"/>
+      <c r="AA21" s="91"/>
       <c r="AB21" s="7"/>
-      <c r="AC21" s="88">
+      <c r="AC21" s="93">
         <v>52.0</v>
       </c>
       <c r="AD21" s="17"/>
@@ -2210,13 +2343,13 @@
         <v>19.0</v>
       </c>
       <c r="AJ21" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AK21" s="1">
         <v>51.0</v>
       </c>
       <c r="AL21" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AT21" s="2"/>
     </row>
@@ -2228,36 +2361,38 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="80">
+        <v>63.0</v>
+      </c>
       <c r="J22" s="16"/>
-      <c r="K22" s="89"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="90"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="95"/>
       <c r="N22" s="21"/>
-      <c r="O22" s="40"/>
+      <c r="O22" s="41"/>
       <c r="P22" s="7"/>
-      <c r="Q22" s="91"/>
-      <c r="R22" s="92"/>
-      <c r="S22" s="93">
+      <c r="Q22" s="96"/>
+      <c r="R22" s="97"/>
+      <c r="S22" s="98">
         <v>46.0</v>
       </c>
       <c r="T22" s="7"/>
-      <c r="U22" s="88">
+      <c r="U22" s="93">
         <v>48.0</v>
       </c>
       <c r="V22" s="7"/>
-      <c r="W22" s="94">
+      <c r="W22" s="99">
         <v>50.0</v>
       </c>
-      <c r="X22" s="46"/>
-      <c r="Y22" s="95">
+      <c r="X22" s="47"/>
+      <c r="Y22" s="100">
         <v>53.0</v>
       </c>
-      <c r="Z22" s="46"/>
-      <c r="AA22" s="87"/>
+      <c r="Z22" s="47"/>
+      <c r="AA22" s="92"/>
       <c r="AB22" s="7"/>
-      <c r="AC22" s="96">
+      <c r="AC22" s="101">
         <v>54.0</v>
       </c>
       <c r="AD22" s="17"/>
@@ -2269,13 +2404,13 @@
         <v>20.0</v>
       </c>
       <c r="AJ22" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AK22" s="1">
         <v>52.0</v>
       </c>
       <c r="AL22" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AT22" s="2"/>
     </row>
@@ -2287,32 +2422,34 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="69"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
-      <c r="M23" s="97">
+      <c r="M23" s="102">
         <v>17.0</v>
       </c>
-      <c r="N23" s="7"/>
+      <c r="N23" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
-      <c r="Q23" s="98"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
-      <c r="T23" s="46"/>
-      <c r="U23" s="88"/>
+      <c r="Q23" s="103"/>
+      <c r="R23" s="47"/>
+      <c r="S23" s="47"/>
+      <c r="T23" s="47"/>
+      <c r="U23" s="93"/>
       <c r="V23" s="7"/>
-      <c r="W23" s="88">
+      <c r="W23" s="93">
         <v>49.0</v>
       </c>
-      <c r="X23" s="46"/>
-      <c r="Y23" s="99" t="s">
-        <v>52</v>
+      <c r="X23" s="47"/>
+      <c r="Y23" s="104" t="s">
+        <v>55</v>
       </c>
-      <c r="Z23" s="46"/>
-      <c r="AA23" s="87"/>
+      <c r="Z23" s="105"/>
+      <c r="AA23" s="92"/>
       <c r="AB23" s="7"/>
       <c r="AC23" s="7"/>
       <c r="AD23" s="7"/>
@@ -2324,13 +2461,13 @@
         <v>21.0</v>
       </c>
       <c r="AJ23" s="6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AK23" s="1">
         <v>53.0</v>
       </c>
       <c r="AL23" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
@@ -2348,32 +2485,32 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="100"/>
-      <c r="K24" s="100"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="106"/>
+      <c r="J24" s="107"/>
+      <c r="K24" s="108"/>
       <c r="L24" s="7"/>
-      <c r="M24" s="47"/>
+      <c r="M24" s="48"/>
       <c r="N24" s="7"/>
-      <c r="O24" s="91">
+      <c r="O24" s="96">
         <v>47.0</v>
       </c>
-      <c r="P24" s="92"/>
-      <c r="Q24" s="101"/>
-      <c r="R24" s="46"/>
-      <c r="S24" s="102"/>
-      <c r="T24" s="80"/>
-      <c r="U24" s="103"/>
-      <c r="V24" s="80"/>
-      <c r="W24" s="104"/>
-      <c r="X24" s="46"/>
-      <c r="Y24" s="95"/>
-      <c r="Z24" s="46"/>
-      <c r="AA24" s="105"/>
-      <c r="AB24" s="106">
+      <c r="P24" s="97"/>
+      <c r="Q24" s="109"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="110"/>
+      <c r="T24" s="85"/>
+      <c r="U24" s="111"/>
+      <c r="V24" s="85"/>
+      <c r="W24" s="112"/>
+      <c r="X24" s="47"/>
+      <c r="Y24" s="100"/>
+      <c r="Z24" s="47"/>
+      <c r="AA24" s="113"/>
+      <c r="AB24" s="114">
         <v>56.0</v>
       </c>
-      <c r="AC24" s="107"/>
+      <c r="AC24" s="115"/>
       <c r="AD24" s="17"/>
       <c r="AE24" s="7"/>
       <c r="AF24" s="2"/>
@@ -2383,13 +2520,13 @@
         <v>22.0</v>
       </c>
       <c r="AJ24" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AK24" s="1">
         <v>54.0</v>
       </c>
       <c r="AL24" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AT24" s="2"/>
     </row>
@@ -2403,26 +2540,28 @@
       <c r="G25" s="2"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="100"/>
-      <c r="K25" s="108" t="s">
-        <v>57</v>
+      <c r="J25" s="116"/>
+      <c r="K25" s="117" t="s">
+        <v>60</v>
       </c>
       <c r="L25" s="7"/>
-      <c r="M25" s="47"/>
+      <c r="M25" s="48"/>
       <c r="N25" s="7"/>
-      <c r="O25" s="78"/>
+      <c r="O25" s="83"/>
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
-      <c r="S25" s="87"/>
-      <c r="T25" s="46"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="46"/>
-      <c r="W25" s="46"/>
-      <c r="X25" s="46"/>
-      <c r="Y25" s="87"/>
-      <c r="Z25" s="46"/>
-      <c r="AA25" s="87"/>
+      <c r="S25" s="92"/>
+      <c r="T25" s="47"/>
+      <c r="U25" s="105" t="s">
+        <v>61</v>
+      </c>
+      <c r="V25" s="47"/>
+      <c r="W25" s="47"/>
+      <c r="X25" s="47"/>
+      <c r="Y25" s="92"/>
+      <c r="Z25" s="47"/>
+      <c r="AA25" s="92"/>
       <c r="AB25" s="7"/>
       <c r="AC25" s="7"/>
       <c r="AD25" s="7"/>
@@ -2434,13 +2573,13 @@
         <v>23.0</v>
       </c>
       <c r="AJ25" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AK25" s="1">
         <v>55.0</v>
       </c>
       <c r="AL25" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
@@ -2450,33 +2589,35 @@
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="2"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="109"/>
-      <c r="J26" s="54"/>
+      <c r="I26" s="118">
+        <v>62.0</v>
+      </c>
+      <c r="J26" s="55"/>
       <c r="K26" s="21"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="40"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="41"/>
       <c r="N26" s="7"/>
-      <c r="O26" s="110"/>
-      <c r="P26" s="83"/>
-      <c r="Q26" s="83"/>
-      <c r="R26" s="83"/>
-      <c r="S26" s="104"/>
+      <c r="O26" s="119"/>
+      <c r="P26" s="88"/>
+      <c r="Q26" s="88"/>
+      <c r="R26" s="88"/>
+      <c r="S26" s="112"/>
       <c r="T26" s="7"/>
-      <c r="U26" s="111">
+      <c r="U26" s="120">
         <v>61.0</v>
       </c>
-      <c r="V26" s="81">
+      <c r="V26" s="86">
         <v>60.0</v>
       </c>
-      <c r="W26" s="81">
+      <c r="W26" s="86">
         <v>59.0</v>
       </c>
-      <c r="X26" s="80"/>
-      <c r="Y26" s="104"/>
-      <c r="Z26" s="46"/>
-      <c r="AA26" s="112"/>
-      <c r="AB26" s="83"/>
-      <c r="AC26" s="113">
+      <c r="X26" s="85"/>
+      <c r="Y26" s="112"/>
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="121"/>
+      <c r="AB26" s="88"/>
+      <c r="AC26" s="122">
         <v>55.0</v>
       </c>
       <c r="AD26" s="17"/>
@@ -2488,13 +2629,13 @@
         <v>24.0</v>
       </c>
       <c r="AJ26" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AK26" s="1">
         <v>56.0</v>
       </c>
-      <c r="AL26" s="114" t="s">
-        <v>61</v>
+      <c r="AL26" s="123" t="s">
+        <v>65</v>
       </c>
       <c r="AT26" s="2"/>
     </row>
@@ -2513,22 +2654,22 @@
       <c r="L27" s="17"/>
       <c r="M27" s="17"/>
       <c r="N27" s="7"/>
-      <c r="O27" s="115" t="s">
-        <v>62</v>
+      <c r="O27" s="124" t="s">
+        <v>66</v>
       </c>
       <c r="P27" s="17"/>
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
-      <c r="S27" s="116"/>
+      <c r="S27" s="125"/>
       <c r="T27" s="7"/>
-      <c r="U27" s="2"/>
+      <c r="U27" s="126"/>
       <c r="V27" s="17"/>
       <c r="W27" s="17"/>
       <c r="X27" s="17"/>
       <c r="Y27" s="17"/>
       <c r="Z27" s="7"/>
-      <c r="AA27" s="115" t="s">
-        <v>63</v>
+      <c r="AA27" s="124" t="s">
+        <v>67</v>
       </c>
       <c r="AB27" s="17"/>
       <c r="AC27" s="17"/>
@@ -2541,13 +2682,13 @@
         <v>25.0</v>
       </c>
       <c r="AJ27" s="6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AK27" s="1">
         <v>57.0</v>
       </c>
       <c r="AL27" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
@@ -2577,18 +2718,18 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
-      <c r="S28" s="46"/>
-      <c r="T28" s="46"/>
+      <c r="S28" s="47"/>
+      <c r="T28" s="47"/>
       <c r="V28" s="7"/>
-      <c r="W28" s="46"/>
-      <c r="X28" s="46"/>
+      <c r="W28" s="47"/>
+      <c r="X28" s="47"/>
       <c r="Y28" s="7"/>
       <c r="Z28" s="7"/>
       <c r="AA28" s="7"/>
       <c r="AB28" s="7"/>
-      <c r="AC28" s="46"/>
+      <c r="AC28" s="47"/>
       <c r="AD28" s="7"/>
-      <c r="AE28" s="117"/>
+      <c r="AE28" s="127"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
@@ -2596,13 +2737,13 @@
         <v>26.0</v>
       </c>
       <c r="AJ28" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="AK28" s="1">
         <v>58.0</v>
       </c>
       <c r="AL28" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="AM28" s="2"/>
       <c r="AN28" s="2"/>
@@ -2615,8 +2756,12 @@
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="B29" s="128" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="128" t="s">
+        <v>72</v>
+      </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2634,7 +2779,7 @@
       <c r="V29" s="2"/>
       <c r="W29" s="17"/>
       <c r="X29" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
@@ -2649,13 +2794,13 @@
         <v>27.0</v>
       </c>
       <c r="AJ29" s="6" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="AK29" s="1">
         <v>59.0</v>
       </c>
       <c r="AL29" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AM29" s="2"/>
       <c r="AN29" s="2"/>
@@ -2668,19 +2813,18 @@
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="D30" s="118" t="s">
-        <v>52</v>
+      <c r="B30" s="128" t="s">
+        <v>60</v>
       </c>
-      <c r="E30" s="118" t="s">
-        <v>71</v>
+      <c r="C30" s="128" t="s">
+        <v>76</v>
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="V30" s="2"/>
-      <c r="W30" s="62"/>
+      <c r="W30" s="65"/>
       <c r="X30" s="6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
@@ -2696,13 +2840,13 @@
         <v>28.0</v>
       </c>
       <c r="AJ30" s="6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
-      <c r="AK30" s="118">
+      <c r="AK30" s="128">
         <v>60.0</v>
       </c>
-      <c r="AL30" s="118" t="s">
-        <v>74</v>
+      <c r="AL30" s="128" t="s">
+        <v>79</v>
       </c>
       <c r="AM30" s="2"/>
       <c r="AN30" s="2"/>
@@ -2716,18 +2860,12 @@
     <row r="31" ht="13.5" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="D31" s="118" t="s">
-        <v>57</v>
-      </c>
-      <c r="E31" s="118" t="s">
-        <v>75</v>
-      </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="V31" s="2"/>
-      <c r="W31" s="119"/>
+      <c r="W31" s="129"/>
       <c r="X31" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
@@ -2742,13 +2880,13 @@
         <v>29.0</v>
       </c>
       <c r="AJ31" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
-      <c r="AK31" s="118">
+      <c r="AK31" s="128">
         <v>61.0</v>
       </c>
-      <c r="AL31" s="118" t="s">
-        <v>78</v>
+      <c r="AL31" s="128" t="s">
+        <v>82</v>
       </c>
       <c r="AM31" s="2"/>
       <c r="AN31" s="2"/>
@@ -2781,7 +2919,7 @@
       <c r="V32" s="2"/>
       <c r="W32" s="27"/>
       <c r="X32" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
@@ -2796,10 +2934,14 @@
         <v>30.0</v>
       </c>
       <c r="AJ32" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
-      <c r="AK32" s="2"/>
-      <c r="AL32" s="2"/>
+      <c r="AK32" s="1">
+        <v>62.0</v>
+      </c>
+      <c r="AL32" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="AM32" s="2"/>
       <c r="AN32" s="2"/>
       <c r="AO32" s="2"/>
@@ -2811,10 +2953,10 @@
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="B33" s="126"/>
+      <c r="C33" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -2831,9 +2973,9 @@
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
-      <c r="W33" s="120"/>
+      <c r="W33" s="130"/>
       <c r="X33" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
@@ -2849,10 +2991,14 @@
         <v>31.0</v>
       </c>
       <c r="AJ33" s="6" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
-      <c r="AK33" s="2"/>
-      <c r="AL33" s="2"/>
+      <c r="AK33" s="1">
+        <v>63.0</v>
+      </c>
+      <c r="AL33" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="AM33" s="2"/>
       <c r="AN33" s="2"/>
       <c r="AO33" s="2"/>
@@ -2865,9 +3011,9 @@
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="C34" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2884,9 +3030,9 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
-      <c r="W34" s="121"/>
+      <c r="W34" s="131"/>
       <c r="X34" s="1" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
@@ -2902,10 +3048,14 @@
         <v>32.0</v>
       </c>
       <c r="AJ34" s="6" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
-      <c r="AK34" s="2"/>
-      <c r="AL34" s="2"/>
+      <c r="AK34" s="1">
+        <v>64.0</v>
+      </c>
+      <c r="AL34" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="AM34" s="2"/>
       <c r="AN34" s="2"/>
       <c r="AO34" s="2"/>
@@ -2916,13 +3066,19 @@
       <c r="AT34" s="2"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="S35" s="122" t="s">
-        <v>85</v>
+      <c r="S35" s="132"/>
+      <c r="W35" s="133"/>
+      <c r="X35" s="128" t="s">
+        <v>94</v>
       </c>
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
-      <c r="AK35" s="2"/>
-      <c r="AL35" s="2"/>
+      <c r="AK35" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="AL35" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="AM35" s="2"/>
       <c r="AN35" s="2"/>
       <c r="AO35" s="2"/>
@@ -2934,12 +3090,16 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
-      <c r="AK36" s="2"/>
-      <c r="AL36" s="2"/>
+      <c r="AK36" s="1">
+        <v>66.0</v>
+      </c>
+      <c r="AL36" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="AM36" s="2"/>
       <c r="AO36" s="2"/>
       <c r="AP36" s="2"/>
@@ -2950,7 +3110,7 @@
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
@@ -2969,7 +3129,7 @@
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
@@ -2988,7 +3148,7 @@
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
@@ -3007,7 +3167,7 @@
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="AG40" s="2"/>
       <c r="AH40" s="2"/>
@@ -3026,7 +3186,7 @@
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
@@ -3045,7 +3205,7 @@
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
@@ -3063,8 +3223,8 @@
       <c r="AT42" s="2"/>
     </row>
     <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="118" t="s">
-        <v>93</v>
+      <c r="A43" s="128" t="s">
+        <v>104</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3112,8 +3272,8 @@
       <c r="AT43" s="2"/>
     </row>
     <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="118" t="s">
-        <v>94</v>
+      <c r="A44" s="128" t="s">
+        <v>105</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -3156,6 +3316,9 @@
       <c r="AT44" s="2"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
+      <c r="A45" s="128" t="s">
+        <v>106</v>
+      </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -3197,6 +3360,9 @@
       <c r="AT45" s="2"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
+      <c r="A46" s="128" t="s">
+        <v>107</v>
+      </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -3231,7 +3397,7 @@
       <c r="AG46" s="2"/>
       <c r="AH46" s="2"/>
       <c r="AI46" s="1"/>
-      <c r="AJ46" s="65"/>
+      <c r="AJ46" s="68"/>
       <c r="AK46" s="2"/>
       <c r="AL46" s="2"/>
       <c r="AM46" s="2"/>
@@ -3244,6 +3410,9 @@
       <c r="AT46" s="2"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
+      <c r="A47" s="128" t="s">
+        <v>108</v>
+      </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -3754,7 +3923,7 @@
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
       <c r="AI58" s="1"/>
-      <c r="AJ58" s="114"/>
+      <c r="AJ58" s="123"/>
       <c r="AR58" s="2"/>
       <c r="AS58" s="2"/>
       <c r="AT58" s="2"/>
@@ -49073,15 +49242,15 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AJ57:AN57"/>
+    <mergeCell ref="AJ56:AQ56"/>
+    <mergeCell ref="AJ58:AQ58"/>
     <mergeCell ref="AL24:AS24"/>
     <mergeCell ref="AL25:AP25"/>
     <mergeCell ref="AL21:AS21"/>
     <mergeCell ref="AL22:AS22"/>
     <mergeCell ref="AJ53:AQ53"/>
     <mergeCell ref="AJ54:AQ54"/>
-    <mergeCell ref="AJ56:AQ56"/>
-    <mergeCell ref="AJ57:AN57"/>
-    <mergeCell ref="AJ58:AQ58"/>
     <mergeCell ref="AL26:AS26"/>
   </mergeCells>
   <drawing r:id="rId1"/>

</xml_diff>